<commit_message>
adding wholesale discount price to exported pricelist
</commit_message>
<xml_diff>
--- a/docs/masterPriceList.xlsx
+++ b/docs/masterPriceList.xlsx
@@ -1474,7 +1474,7 @@
         <v>22</v>
       </c>
       <c r="J2" s="1">
-        <v>NaN</v>
+        <v>11.7</v>
       </c>
       <c r="K2" s="1">
         <v>11.69</v>
@@ -1533,7 +1533,7 @@
         <v>22</v>
       </c>
       <c r="J3" s="1">
-        <v>NaN</v>
+        <v>11.05</v>
       </c>
       <c r="K3" s="1">
         <v>9.2</v>
@@ -1592,7 +1592,7 @@
         <v>22</v>
       </c>
       <c r="J4" s="1">
-        <v>NaN</v>
+        <v>7.8</v>
       </c>
       <c r="K4" s="1">
         <v>6.49</v>
@@ -1651,7 +1651,7 @@
         <v>22</v>
       </c>
       <c r="J5" s="1">
-        <v>NaN</v>
+        <v>1.63</v>
       </c>
       <c r="K5" s="1">
         <v>5.41</v>
@@ -1710,7 +1710,7 @@
         <v>22</v>
       </c>
       <c r="J6" s="1">
-        <v>NaN</v>
+        <v>11.05</v>
       </c>
       <c r="K6" s="1">
         <v>12.42</v>
@@ -1769,7 +1769,7 @@
         <v>22</v>
       </c>
       <c r="J7" s="1">
-        <v>NaN</v>
+        <v>12.68</v>
       </c>
       <c r="K7" s="1">
         <v>14.25</v>
@@ -1828,7 +1828,7 @@
         <v>22</v>
       </c>
       <c r="J8" s="1">
-        <v>NaN</v>
+        <v>11.05</v>
       </c>
       <c r="K8" s="1">
         <v>25.3</v>
@@ -1887,7 +1887,7 @@
         <v>22</v>
       </c>
       <c r="J9" s="1">
-        <v>NaN</v>
+        <v>12.68</v>
       </c>
       <c r="K9" s="1">
         <v>33.24</v>
@@ -1946,7 +1946,7 @@
         <v>22</v>
       </c>
       <c r="J10" s="1">
-        <v>NaN</v>
+        <v>12.68</v>
       </c>
       <c r="K10" s="1">
         <v>25.28</v>
@@ -2005,7 +2005,7 @@
         <v>22</v>
       </c>
       <c r="J11" s="1">
-        <v>NaN</v>
+        <v>7.8</v>
       </c>
       <c r="K11" s="1">
         <v>0</v>
@@ -2064,7 +2064,7 @@
         <v>22</v>
       </c>
       <c r="J12" s="1">
-        <v>NaN</v>
+        <v>9.43</v>
       </c>
       <c r="K12" s="1">
         <v>19.62</v>
@@ -2123,7 +2123,7 @@
         <v>22</v>
       </c>
       <c r="J13" s="1">
-        <v>NaN</v>
+        <v>9.43</v>
       </c>
       <c r="K13" s="1">
         <v>8.24</v>
@@ -2182,7 +2182,7 @@
         <v>47</v>
       </c>
       <c r="J14" s="1">
-        <v>NaN</v>
+        <v>16.9</v>
       </c>
       <c r="K14" s="1">
         <v>14.07</v>
@@ -2241,7 +2241,7 @@
         <v>47</v>
       </c>
       <c r="J15" s="1">
-        <v>NaN</v>
+        <v>30.88</v>
       </c>
       <c r="K15" s="1">
         <v>25.71</v>
@@ -2300,7 +2300,7 @@
         <v>47</v>
       </c>
       <c r="J16" s="1">
-        <v>NaN</v>
+        <v>11.05</v>
       </c>
       <c r="K16" s="1">
         <v>9.2</v>
@@ -2359,7 +2359,7 @@
         <v>47</v>
       </c>
       <c r="J17" s="1">
-        <v>NaN</v>
+        <v>16.25</v>
       </c>
       <c r="K17" s="1">
         <v>13.53</v>
@@ -2418,7 +2418,7 @@
         <v>47</v>
       </c>
       <c r="J18" s="1">
-        <v>NaN</v>
+        <v>9.1</v>
       </c>
       <c r="K18" s="1">
         <v>7.58</v>
@@ -2477,7 +2477,7 @@
         <v>22</v>
       </c>
       <c r="J19" s="1">
-        <v>NaN</v>
+        <v>16.9</v>
       </c>
       <c r="K19" s="1">
         <v>17.59</v>
@@ -2536,7 +2536,7 @@
         <v>22</v>
       </c>
       <c r="J20" s="1">
-        <v>NaN</v>
+        <v>10.4</v>
       </c>
       <c r="K20" s="1">
         <v>29.44</v>
@@ -2595,7 +2595,7 @@
         <v>47</v>
       </c>
       <c r="J21" s="1">
-        <v>NaN</v>
+        <v>7.15</v>
       </c>
       <c r="K21" s="1">
         <v>5.95</v>
@@ -2654,7 +2654,7 @@
         <v>22</v>
       </c>
       <c r="J22" s="1">
-        <v>NaN</v>
+        <v>16.9</v>
       </c>
       <c r="K22" s="1">
         <v>12.66</v>
@@ -2713,7 +2713,7 @@
         <v>22</v>
       </c>
       <c r="J23" s="1">
-        <v>NaN</v>
+        <v>6.17</v>
       </c>
       <c r="K23" s="1">
         <v>15.42</v>
@@ -2772,7 +2772,7 @@
         <v>22</v>
       </c>
       <c r="J24" s="1">
-        <v>NaN</v>
+        <v>16.9</v>
       </c>
       <c r="K24" s="1">
         <v>12.66</v>
@@ -2831,7 +2831,7 @@
         <v>22</v>
       </c>
       <c r="J25" s="1">
-        <v>NaN</v>
+        <v>16.9</v>
       </c>
       <c r="K25" s="1">
         <v>15.48</v>
@@ -2890,7 +2890,7 @@
         <v>47</v>
       </c>
       <c r="J26" s="1">
-        <v>NaN</v>
+        <v>9.75</v>
       </c>
       <c r="K26" s="1">
         <v>8.12</v>
@@ -2949,7 +2949,7 @@
         <v>22</v>
       </c>
       <c r="J27" s="1">
-        <v>NaN</v>
+        <v>8.45</v>
       </c>
       <c r="K27" s="1">
         <v>11.61</v>
@@ -3008,7 +3008,7 @@
         <v>22</v>
       </c>
       <c r="J28" s="1">
-        <v>NaN</v>
+        <v>12.68</v>
       </c>
       <c r="K28" s="1">
         <v>23.75</v>
@@ -3067,7 +3067,7 @@
         <v>22</v>
       </c>
       <c r="J29" s="1">
-        <v>NaN</v>
+        <v>12.68</v>
       </c>
       <c r="K29" s="1">
         <v>17.94</v>
@@ -3126,7 +3126,7 @@
         <v>22</v>
       </c>
       <c r="J30" s="1">
-        <v>NaN</v>
+        <v>6.83</v>
       </c>
       <c r="K30" s="1">
         <v>0</v>
@@ -3185,7 +3185,7 @@
         <v>22</v>
       </c>
       <c r="J31" s="1">
-        <v>NaN</v>
+        <v>12.03</v>
       </c>
       <c r="K31" s="1">
         <v>10.01</v>
@@ -3244,7 +3244,7 @@
         <v>22</v>
       </c>
       <c r="J32" s="1">
-        <v>NaN</v>
+        <v>27.95</v>
       </c>
       <c r="K32" s="1">
         <v>12.8</v>
@@ -3303,7 +3303,7 @@
         <v>22</v>
       </c>
       <c r="J33" s="1">
-        <v>NaN</v>
+        <v>6.17</v>
       </c>
       <c r="K33" s="1">
         <v>14.14</v>
@@ -3362,7 +3362,7 @@
         <v>22</v>
       </c>
       <c r="J34" s="1">
-        <v>NaN</v>
+        <v>13.65</v>
       </c>
       <c r="K34" s="1">
         <v>23.3</v>
@@ -3421,7 +3421,7 @@
         <v>22</v>
       </c>
       <c r="J35" s="1">
-        <v>NaN</v>
+        <v>10.4</v>
       </c>
       <c r="K35" s="1">
         <v>38.97</v>
@@ -3480,7 +3480,7 @@
         <v>22</v>
       </c>
       <c r="J36" s="1">
-        <v>NaN</v>
+        <v>11.05</v>
       </c>
       <c r="K36" s="1">
         <v>32.16</v>
@@ -3539,7 +3539,7 @@
         <v>22</v>
       </c>
       <c r="J37" s="1">
-        <v>NaN</v>
+        <v>11.7</v>
       </c>
       <c r="K37" s="1">
         <v>25.77</v>
@@ -3598,7 +3598,7 @@
         <v>22</v>
       </c>
       <c r="J38" s="1">
-        <v>NaN</v>
+        <v>10.4</v>
       </c>
       <c r="K38" s="1">
         <v>22.51</v>
@@ -3657,7 +3657,7 @@
         <v>22</v>
       </c>
       <c r="J39" s="1">
-        <v>NaN</v>
+        <v>16.9</v>
       </c>
       <c r="K39" s="1">
         <v>17.59</v>
@@ -3716,7 +3716,7 @@
         <v>22</v>
       </c>
       <c r="J40" s="1">
-        <v>NaN</v>
+        <v>10.08</v>
       </c>
       <c r="K40" s="1">
         <v>8.39</v>
@@ -3775,7 +3775,7 @@
         <v>22</v>
       </c>
       <c r="J41" s="1">
-        <v>NaN</v>
+        <v>16.9</v>
       </c>
       <c r="K41" s="1">
         <v>7.74</v>
@@ -3834,7 +3834,7 @@
         <v>22</v>
       </c>
       <c r="J42" s="1">
-        <v>NaN</v>
+        <v>12.68</v>
       </c>
       <c r="K42" s="1">
         <v>13.72</v>
@@ -3893,7 +3893,7 @@
         <v>22</v>
       </c>
       <c r="J43" s="1">
-        <v>NaN</v>
+        <v>7.8</v>
       </c>
       <c r="K43" s="1">
         <v>6.49</v>
@@ -3952,7 +3952,7 @@
         <v>22</v>
       </c>
       <c r="J44" s="1">
-        <v>NaN</v>
+        <v>24.05</v>
       </c>
       <c r="K44" s="1">
         <v>14.02</v>
@@ -4011,7 +4011,7 @@
         <v>22</v>
       </c>
       <c r="J45" s="1">
-        <v>NaN</v>
+        <v>7.8</v>
       </c>
       <c r="K45" s="1">
         <v>6.49</v>
@@ -4070,7 +4070,7 @@
         <v>22</v>
       </c>
       <c r="J46" s="1">
-        <v>NaN</v>
+        <v>26.32</v>
       </c>
       <c r="K46" s="1">
         <v>20.82</v>
@@ -4129,7 +4129,7 @@
         <v>22</v>
       </c>
       <c r="J47" s="1">
-        <v>NaN</v>
+        <v>16.9</v>
       </c>
       <c r="K47" s="1">
         <v>14.07</v>
@@ -4188,7 +4188,7 @@
         <v>22</v>
       </c>
       <c r="J48" s="1">
-        <v>NaN</v>
+        <v>16.9</v>
       </c>
       <c r="K48" s="1">
         <v>8.37</v>
@@ -4247,7 +4247,7 @@
         <v>22</v>
       </c>
       <c r="J49" s="1">
-        <v>NaN</v>
+        <v>16.9</v>
       </c>
       <c r="K49" s="1">
         <v>7.74</v>
@@ -4306,7 +4306,7 @@
         <v>22</v>
       </c>
       <c r="J50" s="1">
-        <v>NaN</v>
+        <v>16.25</v>
       </c>
       <c r="K50" s="1">
         <v>19.62</v>
@@ -4365,7 +4365,7 @@
         <v>22</v>
       </c>
       <c r="J51" s="1">
-        <v>NaN</v>
+        <v>3.25</v>
       </c>
       <c r="K51" s="1">
         <v>7.71</v>
@@ -4424,7 +4424,7 @@
         <v>47</v>
       </c>
       <c r="J52" s="1">
-        <v>NaN</v>
+        <v>6.17</v>
       </c>
       <c r="K52" s="1">
         <v>5.14</v>
@@ -4483,7 +4483,7 @@
         <v>47</v>
       </c>
       <c r="J53" s="1">
-        <v>NaN</v>
+        <v>6.17</v>
       </c>
       <c r="K53" s="1">
         <v>5.14</v>
@@ -4542,7 +4542,7 @@
         <v>47</v>
       </c>
       <c r="J54" s="1">
-        <v>NaN</v>
+        <v>7.8</v>
       </c>
       <c r="K54" s="1">
         <v>6.49</v>
@@ -4601,7 +4601,7 @@
         <v>22</v>
       </c>
       <c r="J55" s="1">
-        <v>NaN</v>
+        <v>11.7</v>
       </c>
       <c r="K55" s="1">
         <v>14.61</v>
@@ -4660,7 +4660,7 @@
         <v>22</v>
       </c>
       <c r="J56" s="1">
-        <v>NaN</v>
+        <v>12.03</v>
       </c>
       <c r="K56" s="1">
         <v>63.08</v>
@@ -4719,7 +4719,7 @@
         <v>22</v>
       </c>
       <c r="J57" s="1">
-        <v>NaN</v>
+        <v>10.08</v>
       </c>
       <c r="K57" s="1">
         <v>10.49</v>
@@ -4778,7 +4778,7 @@
         <v>22</v>
       </c>
       <c r="J58" s="1">
-        <v>NaN</v>
+        <v>7.8</v>
       </c>
       <c r="K58" s="1">
         <v>11.37</v>
@@ -4837,7 +4837,7 @@
         <v>22</v>
       </c>
       <c r="J59" s="1">
-        <v>NaN</v>
+        <v>5.85</v>
       </c>
       <c r="K59" s="1">
         <v>26.79</v>
@@ -4896,7 +4896,7 @@
         <v>22</v>
       </c>
       <c r="J60" s="1">
-        <v>NaN</v>
+        <v>6.17</v>
       </c>
       <c r="K60" s="1">
         <v>23.65</v>
@@ -4955,7 +4955,7 @@
         <v>22</v>
       </c>
       <c r="J61" s="1">
-        <v>NaN</v>
+        <v>6.5</v>
       </c>
       <c r="K61" s="1">
         <v>20.02</v>
@@ -5014,7 +5014,7 @@
         <v>22</v>
       </c>
       <c r="J62" s="1">
-        <v>NaN</v>
+        <v>6.83</v>
       </c>
       <c r="K62" s="1">
         <v>16.17</v>
@@ -5073,7 +5073,7 @@
         <v>22</v>
       </c>
       <c r="J63" s="1">
-        <v>NaN</v>
+        <v>7.8</v>
       </c>
       <c r="K63" s="1">
         <v>35.07</v>
@@ -5132,7 +5132,7 @@
         <v>22</v>
       </c>
       <c r="J64" s="1">
-        <v>NaN</v>
+        <v>7.8</v>
       </c>
       <c r="K64" s="1">
         <v>29.55</v>
@@ -5191,7 +5191,7 @@
         <v>22</v>
       </c>
       <c r="J65" s="1">
-        <v>NaN</v>
+        <v>7.8</v>
       </c>
       <c r="K65" s="1">
         <v>22.73</v>
@@ -5250,7 +5250,7 @@
         <v>47</v>
       </c>
       <c r="J66" s="1">
-        <v>NaN</v>
+        <v>12.03</v>
       </c>
       <c r="K66" s="1">
         <v>10.01</v>
@@ -5309,7 +5309,7 @@
         <v>47</v>
       </c>
       <c r="J67" s="1">
-        <v>NaN</v>
+        <v>7.8</v>
       </c>
       <c r="K67" s="1">
         <v>6.49</v>
@@ -5368,7 +5368,7 @@
         <v>22</v>
       </c>
       <c r="J68" s="1">
-        <v>NaN</v>
+        <v>13</v>
       </c>
       <c r="K68" s="1">
         <v>10.82</v>
@@ -5427,7 +5427,7 @@
         <v>22</v>
       </c>
       <c r="J69" s="1">
-        <v>NaN</v>
+        <v>1.63</v>
       </c>
       <c r="K69" s="1">
         <v>5.41</v>
@@ -5486,7 +5486,7 @@
         <v>22</v>
       </c>
       <c r="J70" s="1">
-        <v>NaN</v>
+        <v>15.6</v>
       </c>
       <c r="K70" s="1">
         <v>11.69</v>
@@ -5545,7 +5545,7 @@
         <v>22</v>
       </c>
       <c r="J71" s="1">
-        <v>NaN</v>
+        <v>15.6</v>
       </c>
       <c r="K71" s="1">
         <v>22.73</v>
@@ -5604,7 +5604,7 @@
         <v>22</v>
       </c>
       <c r="J72" s="1">
-        <v>NaN</v>
+        <v>6.17</v>
       </c>
       <c r="K72" s="1">
         <v>4.88</v>
@@ -5663,7 +5663,7 @@
         <v>22</v>
       </c>
       <c r="J73" s="1">
-        <v>NaN</v>
+        <v>13.97</v>
       </c>
       <c r="K73" s="1">
         <v>14.25</v>
@@ -5722,7 +5722,7 @@
         <v>22</v>
       </c>
       <c r="J74" s="1">
-        <v>NaN</v>
+        <v>10.08</v>
       </c>
       <c r="K74" s="1">
         <v>10.91</v>
@@ -5781,7 +5781,7 @@
         <v>22</v>
       </c>
       <c r="J75" s="1">
-        <v>NaN</v>
+        <v>12.03</v>
       </c>
       <c r="K75" s="1">
         <v>16.52</v>
@@ -5840,7 +5840,7 @@
         <v>22</v>
       </c>
       <c r="J76" s="1">
-        <v>NaN</v>
+        <v>12.35</v>
       </c>
       <c r="K76" s="1">
         <v>12.85</v>
@@ -5899,7 +5899,7 @@
         <v>22</v>
       </c>
       <c r="J77" s="1">
-        <v>NaN</v>
+        <v>12.35</v>
       </c>
       <c r="K77" s="1">
         <v>23.14</v>
@@ -5958,7 +5958,7 @@
         <v>22</v>
       </c>
       <c r="J78" s="1">
-        <v>NaN</v>
+        <v>13</v>
       </c>
       <c r="K78" s="1">
         <v>27.06</v>
@@ -6017,7 +6017,7 @@
         <v>22</v>
       </c>
       <c r="J79" s="1">
-        <v>NaN</v>
+        <v>8.45</v>
       </c>
       <c r="K79" s="1">
         <v>0</v>
@@ -6076,7 +6076,7 @@
         <v>22</v>
       </c>
       <c r="J80" s="1">
-        <v>NaN</v>
+        <v>13.97</v>
       </c>
       <c r="K80" s="1">
         <v>11.64</v>
@@ -6135,7 +6135,7 @@
         <v>22</v>
       </c>
       <c r="J81" s="1">
-        <v>NaN</v>
+        <v>13.97</v>
       </c>
       <c r="K81" s="1">
         <v>32.58</v>
@@ -6194,7 +6194,7 @@
         <v>47</v>
       </c>
       <c r="J82" s="1">
-        <v>NaN</v>
+        <v>9.43</v>
       </c>
       <c r="K82" s="1">
         <v>7.85</v>
@@ -6253,7 +6253,7 @@
         <v>47</v>
       </c>
       <c r="J83" s="1">
-        <v>NaN</v>
+        <v>11.38</v>
       </c>
       <c r="K83" s="1">
         <v>9.47</v>
@@ -6312,7 +6312,7 @@
         <v>47</v>
       </c>
       <c r="J84" s="1">
-        <v>NaN</v>
+        <v>12.68</v>
       </c>
       <c r="K84" s="1">
         <v>10.55</v>
@@ -6371,7 +6371,7 @@
         <v>47</v>
       </c>
       <c r="J85" s="1">
-        <v>NaN</v>
+        <v>10.08</v>
       </c>
       <c r="K85" s="1">
         <v>8.39</v>
@@ -6430,7 +6430,7 @@
         <v>47</v>
       </c>
       <c r="J86" s="1">
-        <v>NaN</v>
+        <v>12.68</v>
       </c>
       <c r="K86" s="1">
         <v>10.55</v>
@@ -6489,7 +6489,7 @@
         <v>47</v>
       </c>
       <c r="J87" s="1">
-        <v>NaN</v>
+        <v>12.68</v>
       </c>
       <c r="K87" s="1">
         <v>10.55</v>
@@ -6548,7 +6548,7 @@
         <v>47</v>
       </c>
       <c r="J88" s="1">
-        <v>NaN</v>
+        <v>13.97</v>
       </c>
       <c r="K88" s="1">
         <v>11.64</v>
@@ -6607,7 +6607,7 @@
         <v>47</v>
       </c>
       <c r="J89" s="1">
-        <v>NaN</v>
+        <v>13.97</v>
       </c>
       <c r="K89" s="1">
         <v>11.64</v>
@@ -6666,7 +6666,7 @@
         <v>47</v>
       </c>
       <c r="J90" s="1">
-        <v>NaN</v>
+        <v>10.72</v>
       </c>
       <c r="K90" s="1">
         <v>8.93</v>
@@ -6725,7 +6725,7 @@
         <v>47</v>
       </c>
       <c r="J91" s="1">
-        <v>NaN</v>
+        <v>13</v>
       </c>
       <c r="K91" s="1">
         <v>10.82</v>
@@ -6784,7 +6784,7 @@
         <v>47</v>
       </c>
       <c r="J92" s="1">
-        <v>NaN</v>
+        <v>13.97</v>
       </c>
       <c r="K92" s="1">
         <v>11.64</v>
@@ -6843,7 +6843,7 @@
         <v>47</v>
       </c>
       <c r="J93" s="1">
-        <v>NaN</v>
+        <v>11.7</v>
       </c>
       <c r="K93" s="1">
         <v>9.74</v>
@@ -6902,7 +6902,7 @@
         <v>47</v>
       </c>
       <c r="J94" s="1">
-        <v>NaN</v>
+        <v>11.7</v>
       </c>
       <c r="K94" s="1">
         <v>9.74</v>
@@ -6961,7 +6961,7 @@
         <v>47</v>
       </c>
       <c r="J95" s="1">
-        <v>NaN</v>
+        <v>13</v>
       </c>
       <c r="K95" s="1">
         <v>10.82</v>
@@ -7020,7 +7020,7 @@
         <v>47</v>
       </c>
       <c r="J96" s="1">
-        <v>NaN</v>
+        <v>11.7</v>
       </c>
       <c r="K96" s="1">
         <v>9.74</v>
@@ -7079,7 +7079,7 @@
         <v>47</v>
       </c>
       <c r="J97" s="1">
-        <v>NaN</v>
+        <v>13</v>
       </c>
       <c r="K97" s="1">
         <v>10.82</v>
@@ -7138,7 +7138,7 @@
         <v>47</v>
       </c>
       <c r="J98" s="1">
-        <v>NaN</v>
+        <v>5.85</v>
       </c>
       <c r="K98" s="1">
         <v>4.87</v>
@@ -7197,7 +7197,7 @@
         <v>47</v>
       </c>
       <c r="J99" s="1">
-        <v>NaN</v>
+        <v>12.68</v>
       </c>
       <c r="K99" s="1">
         <v>10.55</v>
@@ -7256,7 +7256,7 @@
         <v>47</v>
       </c>
       <c r="J100" s="1">
-        <v>NaN</v>
+        <v>13</v>
       </c>
       <c r="K100" s="1">
         <v>10.82</v>
@@ -7315,7 +7315,7 @@
         <v>47</v>
       </c>
       <c r="J101" s="1">
-        <v>NaN</v>
+        <v>10.72</v>
       </c>
       <c r="K101" s="1">
         <v>8.93</v>
@@ -7374,7 +7374,7 @@
         <v>47</v>
       </c>
       <c r="J102" s="1">
-        <v>NaN</v>
+        <v>7.15</v>
       </c>
       <c r="K102" s="1">
         <v>5.95</v>
@@ -7433,7 +7433,7 @@
         <v>47</v>
       </c>
       <c r="J103" s="1">
-        <v>NaN</v>
+        <v>11.05</v>
       </c>
       <c r="K103" s="1">
         <v>9.2</v>
@@ -7492,7 +7492,7 @@
         <v>47</v>
       </c>
       <c r="J104" s="1">
-        <v>NaN</v>
+        <v>12.68</v>
       </c>
       <c r="K104" s="1">
         <v>10.55</v>
@@ -7551,7 +7551,7 @@
         <v>47</v>
       </c>
       <c r="J105" s="1">
-        <v>NaN</v>
+        <v>11.7</v>
       </c>
       <c r="K105" s="1">
         <v>9.74</v>
@@ -7610,7 +7610,7 @@
         <v>47</v>
       </c>
       <c r="J106" s="1">
-        <v>NaN</v>
+        <v>7.8</v>
       </c>
       <c r="K106" s="1">
         <v>6.49</v>
@@ -7669,7 +7669,7 @@
         <v>47</v>
       </c>
       <c r="J107" s="1">
-        <v>NaN</v>
+        <v>4.55</v>
       </c>
       <c r="K107" s="1">
         <v>3.79</v>
@@ -7728,7 +7728,7 @@
         <v>47</v>
       </c>
       <c r="J108" s="1">
-        <v>NaN</v>
+        <v>13</v>
       </c>
       <c r="K108" s="1">
         <v>10.82</v>
@@ -7787,7 +7787,7 @@
         <v>47</v>
       </c>
       <c r="J109" s="1">
-        <v>NaN</v>
+        <v>10.72</v>
       </c>
       <c r="K109" s="1">
         <v>8.93</v>
@@ -7846,7 +7846,7 @@
         <v>47</v>
       </c>
       <c r="J110" s="1">
-        <v>NaN</v>
+        <v>10.72</v>
       </c>
       <c r="K110" s="1">
         <v>8.93</v>
@@ -7905,7 +7905,7 @@
         <v>47</v>
       </c>
       <c r="J111" s="1">
-        <v>NaN</v>
+        <v>10.72</v>
       </c>
       <c r="K111" s="1">
         <v>8.93</v>
@@ -7964,7 +7964,7 @@
         <v>47</v>
       </c>
       <c r="J112" s="1">
-        <v>NaN</v>
+        <v>11.05</v>
       </c>
       <c r="K112" s="1">
         <v>9.2</v>
@@ -8023,7 +8023,7 @@
         <v>47</v>
       </c>
       <c r="J113" s="1">
-        <v>NaN</v>
+        <v>10.72</v>
       </c>
       <c r="K113" s="1">
         <v>8.93</v>
@@ -8082,7 +8082,7 @@
         <v>47</v>
       </c>
       <c r="J114" s="1">
-        <v>NaN</v>
+        <v>13</v>
       </c>
       <c r="K114" s="1">
         <v>10.82</v>
@@ -8141,7 +8141,7 @@
         <v>47</v>
       </c>
       <c r="J115" s="1">
-        <v>NaN</v>
+        <v>13</v>
       </c>
       <c r="K115" s="1">
         <v>10.82</v>
@@ -8200,7 +8200,7 @@
         <v>47</v>
       </c>
       <c r="J116" s="1">
-        <v>NaN</v>
+        <v>13</v>
       </c>
       <c r="K116" s="1">
         <v>10.82</v>
@@ -8259,7 +8259,7 @@
         <v>47</v>
       </c>
       <c r="J117" s="1">
-        <v>NaN</v>
+        <v>13</v>
       </c>
       <c r="K117" s="1">
         <v>10.82</v>
@@ -8318,7 +8318,7 @@
         <v>47</v>
       </c>
       <c r="J118" s="1">
-        <v>NaN</v>
+        <v>9.75</v>
       </c>
       <c r="K118" s="1">
         <v>8.12</v>
@@ -8377,7 +8377,7 @@
         <v>47</v>
       </c>
       <c r="J119" s="1">
-        <v>NaN</v>
+        <v>13</v>
       </c>
       <c r="K119" s="1">
         <v>10.82</v>
@@ -8436,7 +8436,7 @@
         <v>47</v>
       </c>
       <c r="J120" s="1">
-        <v>NaN</v>
+        <v>13</v>
       </c>
       <c r="K120" s="1">
         <v>10.82</v>
@@ -8495,7 +8495,7 @@
         <v>47</v>
       </c>
       <c r="J121" s="1">
-        <v>NaN</v>
+        <v>15.6</v>
       </c>
       <c r="K121" s="1">
         <v>12.99</v>
@@ -8554,7 +8554,7 @@
         <v>47</v>
       </c>
       <c r="J122" s="1">
-        <v>NaN</v>
+        <v>13</v>
       </c>
       <c r="K122" s="1">
         <v>10.82</v>
@@ -8613,7 +8613,7 @@
         <v>47</v>
       </c>
       <c r="J123" s="1">
-        <v>NaN</v>
+        <v>6.5</v>
       </c>
       <c r="K123" s="1">
         <v>5.41</v>
@@ -8672,7 +8672,7 @@
         <v>47</v>
       </c>
       <c r="J124" s="1">
-        <v>NaN</v>
+        <v>9.75</v>
       </c>
       <c r="K124" s="1">
         <v>8.12</v>
@@ -8731,7 +8731,7 @@
         <v>47</v>
       </c>
       <c r="J125" s="1">
-        <v>NaN</v>
+        <v>6.5</v>
       </c>
       <c r="K125" s="1">
         <v>5.41</v>
@@ -8790,7 +8790,7 @@
         <v>47</v>
       </c>
       <c r="J126" s="1">
-        <v>NaN</v>
+        <v>10.4</v>
       </c>
       <c r="K126" s="1">
         <v>8.66</v>
@@ -8849,7 +8849,7 @@
         <v>47</v>
       </c>
       <c r="J127" s="1">
-        <v>NaN</v>
+        <v>6.5</v>
       </c>
       <c r="K127" s="1">
         <v>5.41</v>
@@ -8908,7 +8908,7 @@
         <v>47</v>
       </c>
       <c r="J128" s="1">
-        <v>NaN</v>
+        <v>14.3</v>
       </c>
       <c r="K128" s="1">
         <v>11.91</v>
@@ -8967,7 +8967,7 @@
         <v>47</v>
       </c>
       <c r="J129" s="1">
-        <v>NaN</v>
+        <v>13</v>
       </c>
       <c r="K129" s="1">
         <v>10.82</v>

</xml_diff>

<commit_message>
updating products to account for dairy
</commit_message>
<xml_diff>
--- a/docs/masterPriceList.xlsx
+++ b/docs/masterPriceList.xlsx
@@ -2293,13 +2293,13 @@
         <v>50</v>
       </c>
       <c r="Q12" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="R12">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="S12" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -2355,7 +2355,7 @@
         <v>23</v>
       </c>
       <c r="R13">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="S13" t="s">
         <v>23</v>
@@ -2709,7 +2709,7 @@
         <v>23</v>
       </c>
       <c r="R19">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="S19" t="s">
         <v>23</v>
@@ -2768,7 +2768,7 @@
         <v>23</v>
       </c>
       <c r="R20">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S20" t="s">
         <v>23</v>
@@ -2883,13 +2883,13 @@
         <v>76</v>
       </c>
       <c r="Q22" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="R22">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="S22" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
@@ -3122,7 +3122,7 @@
         <v>23</v>
       </c>
       <c r="R26">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="S26" t="s">
         <v>23</v>
@@ -3178,13 +3178,13 @@
         <v>89</v>
       </c>
       <c r="Q27" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="R27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S27" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
@@ -3476,7 +3476,7 @@
         <v>23</v>
       </c>
       <c r="R32">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="S32" t="s">
         <v>23</v>
@@ -3535,7 +3535,7 @@
         <v>23</v>
       </c>
       <c r="R33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S33" t="s">
         <v>23</v>
@@ -3650,13 +3650,13 @@
         <v>19</v>
       </c>
       <c r="Q35" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="R35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S35" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
@@ -3712,7 +3712,7 @@
         <v>23</v>
       </c>
       <c r="R36">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S36" t="s">
         <v>23</v>
@@ -3768,13 +3768,13 @@
         <v>19</v>
       </c>
       <c r="Q37" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="R37">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S37" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
@@ -3830,7 +3830,7 @@
         <v>23</v>
       </c>
       <c r="R38">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="S38" t="s">
         <v>23</v>
@@ -3886,13 +3886,13 @@
         <v>117</v>
       </c>
       <c r="Q39" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="R39">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="S39" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
@@ -4004,13 +4004,13 @@
         <v>121</v>
       </c>
       <c r="Q41" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="R41">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S41" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
@@ -4181,13 +4181,13 @@
         <v>19</v>
       </c>
       <c r="Q44" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="R44">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="S44" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
@@ -4302,7 +4302,7 @@
         <v>23</v>
       </c>
       <c r="R46">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="S46" t="s">
         <v>23</v>
@@ -4358,13 +4358,13 @@
         <v>135</v>
       </c>
       <c r="Q47" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="R47">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="S47" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
@@ -4417,13 +4417,13 @@
         <v>135</v>
       </c>
       <c r="Q48" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="R48">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="S48" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
@@ -4476,13 +4476,13 @@
         <v>139</v>
       </c>
       <c r="Q49" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="R49">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="S49" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
@@ -4538,7 +4538,7 @@
         <v>23</v>
       </c>
       <c r="R50">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="S50" t="s">
         <v>23</v>
@@ -5656,13 +5656,13 @@
         <v>190</v>
       </c>
       <c r="Q69" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="R69">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S69" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.25">
@@ -5836,7 +5836,7 @@
         <v>23</v>
       </c>
       <c r="R72">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="S72" t="s">
         <v>23</v>
@@ -8370,13 +8370,13 @@
         <v>19</v>
       </c>
       <c r="Q115" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="R115">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S115" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="116" spans="1:19" x14ac:dyDescent="0.25">
@@ -9918,7 +9918,7 @@
         <v>164</v>
       </c>
       <c r="B142">
-        <v>999998</v>
+        <v>990715</v>
       </c>
       <c r="C142" t="s">
         <v>19</v>
@@ -10685,7 +10685,7 @@
         <v>165</v>
       </c>
       <c r="B155">
-        <v>999999</v>
+        <v>990712</v>
       </c>
       <c r="C155" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Updating master pricelist to adjust pricing
</commit_message>
<xml_diff>
--- a/docs/masterPriceList.xlsx
+++ b/docs/masterPriceList.xlsx
@@ -5,13 +5,14 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="Pricelist" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Variables" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="392">
   <si>
     <t>id</t>
   </si>
@@ -1201,6 +1202,24 @@
   <si>
     <t xml:space="preserve">This thick, rich sour cream is perfect to dollop onto soups or into spicy burritos!
 Purchase of raw dairy products requires you to agree to our product liability agreement  . </t>
+  </si>
+  <si>
+    <t>values</t>
+  </si>
+  <si>
+    <t>keys</t>
+  </si>
+  <si>
+    <t>DISCOUNT</t>
+  </si>
+  <si>
+    <t>WHOLESALE_DISCOUNT</t>
+  </si>
+  <si>
+    <t>MEMBER_MARKUP</t>
+  </si>
+  <si>
+    <t>GUEST_MARKUP</t>
   </si>
 </sst>
 </file>
@@ -10920,4 +10939,55 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>386</v>
+      </c>
+      <c r="B1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.5412</v>
+      </c>
+      <c r="B2" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.6574</v>
+      </c>
+      <c r="B4" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.8496</v>
+      </c>
+      <c r="B5" t="s">
+        <v>391</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updating all products with new guest pricing
</commit_message>
<xml_diff>
--- a/docs/masterPriceList.xlsx
+++ b/docs/masterPriceList.xlsx
@@ -1710,7 +1710,7 @@
         <v>19.37</v>
       </c>
       <c r="M2" s="1">
-        <v>21.62</v>
+        <v>22.21</v>
       </c>
       <c r="N2">
         <v>1</v>
@@ -1769,7 +1769,7 @@
         <v>15.25</v>
       </c>
       <c r="M3" s="1">
-        <v>17.02</v>
+        <v>17.48</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -1828,7 +1828,7 @@
         <v>10.76</v>
       </c>
       <c r="M4" s="1">
-        <v>12.01</v>
+        <v>12.34</v>
       </c>
       <c r="N4">
         <v>1</v>
@@ -1887,7 +1887,7 @@
         <v>8.97</v>
       </c>
       <c r="M5" s="1">
-        <v>10.01</v>
+        <v>10.28</v>
       </c>
       <c r="N5">
         <v>1</v>
@@ -1946,7 +1946,7 @@
         <v>20.59</v>
       </c>
       <c r="M6" s="1">
-        <v>22.97</v>
+        <v>23.6</v>
       </c>
       <c r="N6">
         <v>1</v>
@@ -2005,7 +2005,7 @@
         <v>23.61</v>
       </c>
       <c r="M7" s="1">
-        <v>26.35</v>
+        <v>27.07</v>
       </c>
       <c r="N7">
         <v>1</v>
@@ -2064,7 +2064,7 @@
         <v>41.93</v>
       </c>
       <c r="M8" s="1">
-        <v>46.8</v>
+        <v>48.07</v>
       </c>
       <c r="N8">
         <v>1</v>
@@ -2123,7 +2123,7 @@
         <v>55.1</v>
       </c>
       <c r="M9" s="1">
-        <v>61.49</v>
+        <v>63.16</v>
       </c>
       <c r="N9">
         <v>1</v>
@@ -2182,7 +2182,7 @@
         <v>41.89</v>
       </c>
       <c r="M10" s="1">
-        <v>46.75</v>
+        <v>48.02</v>
       </c>
       <c r="N10">
         <v>1</v>
@@ -2300,7 +2300,7 @@
         <v>32.52</v>
       </c>
       <c r="M12" s="1">
-        <v>36.29</v>
+        <v>37.28</v>
       </c>
       <c r="N12">
         <v>1</v>
@@ -2359,7 +2359,7 @@
         <v>13.66</v>
       </c>
       <c r="M13" s="1">
-        <v>15.24</v>
+        <v>15.66</v>
       </c>
       <c r="N13">
         <v>1</v>
@@ -2418,7 +2418,7 @@
         <v>23.32</v>
       </c>
       <c r="M14" s="1">
-        <v>26.03</v>
+        <v>26.74</v>
       </c>
       <c r="N14">
         <v>1</v>
@@ -2477,7 +2477,7 @@
         <v>42.61</v>
       </c>
       <c r="M15" s="1">
-        <v>47.55</v>
+        <v>48.84</v>
       </c>
       <c r="N15">
         <v>1</v>
@@ -2536,7 +2536,7 @@
         <v>15.25</v>
       </c>
       <c r="M16" s="1">
-        <v>17.02</v>
+        <v>17.48</v>
       </c>
       <c r="N16">
         <v>1</v>
@@ -2595,7 +2595,7 @@
         <v>22.42</v>
       </c>
       <c r="M17" s="1">
-        <v>25.03</v>
+        <v>25.71</v>
       </c>
       <c r="N17">
         <v>1</v>
@@ -2654,7 +2654,7 @@
         <v>12.56</v>
       </c>
       <c r="M18" s="1">
-        <v>14.01</v>
+        <v>14.4</v>
       </c>
       <c r="N18">
         <v>1</v>
@@ -2713,7 +2713,7 @@
         <v>29.15</v>
       </c>
       <c r="M19" s="1">
-        <v>32.53</v>
+        <v>33.42</v>
       </c>
       <c r="N19">
         <v>1</v>
@@ -2772,7 +2772,7 @@
         <v>48.8</v>
       </c>
       <c r="M20" s="1">
-        <v>54.45</v>
+        <v>55.94</v>
       </c>
       <c r="N20">
         <v>1</v>
@@ -2831,7 +2831,7 @@
         <v>9.87</v>
       </c>
       <c r="M21" s="1">
-        <v>11.01</v>
+        <v>11.31</v>
       </c>
       <c r="N21">
         <v>1</v>
@@ -2890,7 +2890,7 @@
         <v>20.99</v>
       </c>
       <c r="M22" s="1">
-        <v>23.42</v>
+        <v>24.06</v>
       </c>
       <c r="N22">
         <v>1</v>
@@ -2949,7 +2949,7 @@
         <v>25.56</v>
       </c>
       <c r="M23" s="1">
-        <v>28.53</v>
+        <v>29.31</v>
       </c>
       <c r="N23">
         <v>1</v>
@@ -3008,7 +3008,7 @@
         <v>20.99</v>
       </c>
       <c r="M24" s="1">
-        <v>23.42</v>
+        <v>24.06</v>
       </c>
       <c r="N24">
         <v>1</v>
@@ -3067,7 +3067,7 @@
         <v>25.65</v>
       </c>
       <c r="M25" s="1">
-        <v>28.63</v>
+        <v>29.41</v>
       </c>
       <c r="N25">
         <v>1</v>
@@ -3126,7 +3126,7 @@
         <v>13.45</v>
       </c>
       <c r="M26" s="1">
-        <v>15.02</v>
+        <v>15.42</v>
       </c>
       <c r="N26">
         <v>1</v>
@@ -3185,7 +3185,7 @@
         <v>19.24</v>
       </c>
       <c r="M27" s="1">
-        <v>21.47</v>
+        <v>22.06</v>
       </c>
       <c r="N27">
         <v>1</v>
@@ -3244,7 +3244,7 @@
         <v>39.36</v>
       </c>
       <c r="M28" s="1">
-        <v>43.92</v>
+        <v>45.12</v>
       </c>
       <c r="N28">
         <v>1</v>
@@ -3303,7 +3303,7 @@
         <v>29.74</v>
       </c>
       <c r="M29" s="1">
-        <v>33.18</v>
+        <v>34.09</v>
       </c>
       <c r="N29">
         <v>1</v>
@@ -3421,7 +3421,7 @@
         <v>16.59</v>
       </c>
       <c r="M31" s="1">
-        <v>18.52</v>
+        <v>19.02</v>
       </c>
       <c r="N31">
         <v>1</v>
@@ -3480,7 +3480,7 @@
         <v>21.21</v>
       </c>
       <c r="M32" s="1">
-        <v>23.67</v>
+        <v>24.32</v>
       </c>
       <c r="N32">
         <v>1</v>
@@ -3539,7 +3539,7 @@
         <v>23.43</v>
       </c>
       <c r="M33" s="1">
-        <v>26.15</v>
+        <v>26.86</v>
       </c>
       <c r="N33">
         <v>1</v>
@@ -3598,7 +3598,7 @@
         <v>38.62</v>
       </c>
       <c r="M34" s="1">
-        <v>43.09</v>
+        <v>44.27</v>
       </c>
       <c r="N34">
         <v>1</v>
@@ -3657,7 +3657,7 @@
         <v>64.58</v>
       </c>
       <c r="M35" s="1">
-        <v>72.07</v>
+        <v>74.04</v>
       </c>
       <c r="N35">
         <v>1</v>
@@ -3716,7 +3716,7 @@
         <v>53.29</v>
       </c>
       <c r="M36" s="1">
-        <v>59.47</v>
+        <v>61.1</v>
       </c>
       <c r="N36">
         <v>1</v>
@@ -3775,7 +3775,7 @@
         <v>42.71</v>
       </c>
       <c r="M37" s="1">
-        <v>47.66</v>
+        <v>48.96</v>
       </c>
       <c r="N37">
         <v>1</v>
@@ -3834,7 +3834,7 @@
         <v>37.31</v>
       </c>
       <c r="M38" s="1">
-        <v>41.64</v>
+        <v>42.78</v>
       </c>
       <c r="N38">
         <v>1</v>
@@ -3893,7 +3893,7 @@
         <v>29.15</v>
       </c>
       <c r="M39" s="1">
-        <v>32.53</v>
+        <v>33.42</v>
       </c>
       <c r="N39">
         <v>1</v>
@@ -3952,7 +3952,7 @@
         <v>13.9</v>
       </c>
       <c r="M40" s="1">
-        <v>15.52</v>
+        <v>15.94</v>
       </c>
       <c r="N40">
         <v>1</v>
@@ -4011,7 +4011,7 @@
         <v>12.83</v>
       </c>
       <c r="M41" s="1">
-        <v>14.31</v>
+        <v>14.7</v>
       </c>
       <c r="N41">
         <v>1</v>
@@ -4070,7 +4070,7 @@
         <v>22.74</v>
       </c>
       <c r="M42" s="1">
-        <v>25.38</v>
+        <v>26.07</v>
       </c>
       <c r="N42">
         <v>1</v>
@@ -4129,7 +4129,7 @@
         <v>10.76</v>
       </c>
       <c r="M43" s="1">
-        <v>12.01</v>
+        <v>12.34</v>
       </c>
       <c r="N43">
         <v>1</v>
@@ -4188,7 +4188,7 @@
         <v>23.23</v>
       </c>
       <c r="M44" s="1">
-        <v>25.93</v>
+        <v>26.63</v>
       </c>
       <c r="N44">
         <v>1</v>
@@ -4247,7 +4247,7 @@
         <v>10.76</v>
       </c>
       <c r="M45" s="1">
-        <v>12.01</v>
+        <v>12.34</v>
       </c>
       <c r="N45">
         <v>1</v>
@@ -4306,7 +4306,7 @@
         <v>34.51</v>
       </c>
       <c r="M46" s="1">
-        <v>38.51</v>
+        <v>39.56</v>
       </c>
       <c r="N46">
         <v>1</v>
@@ -4365,7 +4365,7 @@
         <v>23.32</v>
       </c>
       <c r="M47" s="1">
-        <v>26.03</v>
+        <v>26.74</v>
       </c>
       <c r="N47">
         <v>1</v>
@@ -4424,7 +4424,7 @@
         <v>13.88</v>
       </c>
       <c r="M48" s="1">
-        <v>15.49</v>
+        <v>15.91</v>
       </c>
       <c r="N48">
         <v>1</v>
@@ -4483,7 +4483,7 @@
         <v>12.83</v>
       </c>
       <c r="M49" s="1">
-        <v>14.31</v>
+        <v>14.7</v>
       </c>
       <c r="N49">
         <v>1</v>
@@ -4542,7 +4542,7 @@
         <v>32.52</v>
       </c>
       <c r="M50" s="1">
-        <v>36.29</v>
+        <v>37.28</v>
       </c>
       <c r="N50">
         <v>1</v>
@@ -4601,7 +4601,7 @@
         <v>12.78</v>
       </c>
       <c r="M51" s="1">
-        <v>14.26</v>
+        <v>14.65</v>
       </c>
       <c r="N51">
         <v>1</v>
@@ -4660,7 +4660,7 @@
         <v>8.52</v>
       </c>
       <c r="M52" s="1">
-        <v>9.51</v>
+        <v>9.77</v>
       </c>
       <c r="N52">
         <v>1</v>
@@ -4719,7 +4719,7 @@
         <v>8.52</v>
       </c>
       <c r="M53" s="1">
-        <v>9.51</v>
+        <v>9.77</v>
       </c>
       <c r="N53">
         <v>1</v>
@@ -4778,7 +4778,7 @@
         <v>10.76</v>
       </c>
       <c r="M54" s="1">
-        <v>12.01</v>
+        <v>12.34</v>
       </c>
       <c r="N54">
         <v>1</v>
@@ -4837,7 +4837,7 @@
         <v>24.22</v>
       </c>
       <c r="M55" s="1">
-        <v>27.03</v>
+        <v>27.76</v>
       </c>
       <c r="N55">
         <v>1</v>
@@ -4896,7 +4896,7 @@
         <v>104.54</v>
       </c>
       <c r="M56" s="1">
-        <v>116.67</v>
+        <v>119.85</v>
       </c>
       <c r="N56">
         <v>1</v>
@@ -4955,7 +4955,7 @@
         <v>17.38</v>
       </c>
       <c r="M57" s="1">
-        <v>19.39</v>
+        <v>19.92</v>
       </c>
       <c r="N57">
         <v>1</v>
@@ -5014,7 +5014,7 @@
         <v>18.84</v>
       </c>
       <c r="M58" s="1">
-        <v>21.02</v>
+        <v>21.59</v>
       </c>
       <c r="N58">
         <v>1</v>
@@ -5073,7 +5073,7 @@
         <v>44.4</v>
       </c>
       <c r="M59" s="1">
-        <v>49.55</v>
+        <v>50.9</v>
       </c>
       <c r="N59">
         <v>1</v>
@@ -5132,7 +5132,7 @@
         <v>39.2</v>
       </c>
       <c r="M60" s="1">
-        <v>43.74</v>
+        <v>44.94</v>
       </c>
       <c r="N60">
         <v>1</v>
@@ -5191,7 +5191,7 @@
         <v>33.19</v>
       </c>
       <c r="M61" s="1">
-        <v>37.04</v>
+        <v>38.05</v>
       </c>
       <c r="N61">
         <v>1</v>
@@ -5250,7 +5250,7 @@
         <v>26.8</v>
       </c>
       <c r="M62" s="1">
-        <v>29.9</v>
+        <v>30.72</v>
       </c>
       <c r="N62">
         <v>1</v>
@@ -5309,7 +5309,7 @@
         <v>58.12</v>
       </c>
       <c r="M63" s="1">
-        <v>64.87</v>
+        <v>66.63</v>
       </c>
       <c r="N63">
         <v>1</v>
@@ -5368,7 +5368,7 @@
         <v>48.98</v>
       </c>
       <c r="M64" s="1">
-        <v>54.65</v>
+        <v>56.14</v>
       </c>
       <c r="N64">
         <v>1</v>
@@ -5427,7 +5427,7 @@
         <v>37.67</v>
       </c>
       <c r="M65" s="1">
-        <v>42.04</v>
+        <v>43.19</v>
       </c>
       <c r="N65">
         <v>1</v>
@@ -5486,7 +5486,7 @@
         <v>16.59</v>
       </c>
       <c r="M66" s="1">
-        <v>18.52</v>
+        <v>19.02</v>
       </c>
       <c r="N66">
         <v>1</v>
@@ -5545,7 +5545,7 @@
         <v>10.76</v>
       </c>
       <c r="M67" s="1">
-        <v>12.01</v>
+        <v>12.34</v>
       </c>
       <c r="N67">
         <v>1</v>
@@ -5604,7 +5604,7 @@
         <v>17.94</v>
       </c>
       <c r="M68" s="1">
-        <v>20.02</v>
+        <v>20.57</v>
       </c>
       <c r="N68">
         <v>1</v>
@@ -5663,7 +5663,7 @@
         <v>8.97</v>
       </c>
       <c r="M69" s="1">
-        <v>10.01</v>
+        <v>10.28</v>
       </c>
       <c r="N69">
         <v>1</v>
@@ -5722,7 +5722,7 @@
         <v>19.37</v>
       </c>
       <c r="M70" s="1">
-        <v>21.62</v>
+        <v>22.21</v>
       </c>
       <c r="N70">
         <v>1</v>
@@ -5781,7 +5781,7 @@
         <v>37.67</v>
       </c>
       <c r="M71" s="1">
-        <v>42.04</v>
+        <v>43.19</v>
       </c>
       <c r="N71">
         <v>1</v>
@@ -5840,7 +5840,7 @@
         <v>8.1</v>
       </c>
       <c r="M72" s="1">
-        <v>9.03</v>
+        <v>9.28</v>
       </c>
       <c r="N72">
         <v>1</v>
@@ -5899,7 +5899,7 @@
         <v>23.62</v>
       </c>
       <c r="M73" s="1">
-        <v>26.36</v>
+        <v>27.08</v>
       </c>
       <c r="N73">
         <v>1</v>
@@ -5958,7 +5958,7 @@
         <v>18.07</v>
       </c>
       <c r="M74" s="1">
-        <v>20.17</v>
+        <v>20.72</v>
       </c>
       <c r="N74">
         <v>1</v>
@@ -6017,7 +6017,7 @@
         <v>27.38</v>
       </c>
       <c r="M75" s="1">
-        <v>30.56</v>
+        <v>31.39</v>
       </c>
       <c r="N75">
         <v>1</v>
@@ -6076,7 +6076,7 @@
         <v>21.3</v>
       </c>
       <c r="M76" s="1">
-        <v>23.77</v>
+        <v>24.42</v>
       </c>
       <c r="N76">
         <v>1</v>
@@ -6135,7 +6135,7 @@
         <v>38.35</v>
       </c>
       <c r="M77" s="1">
-        <v>42.79</v>
+        <v>43.96</v>
       </c>
       <c r="N77">
         <v>1</v>
@@ -6194,7 +6194,7 @@
         <v>44.85</v>
       </c>
       <c r="M78" s="1">
-        <v>50.05</v>
+        <v>51.41</v>
       </c>
       <c r="N78">
         <v>1</v>
@@ -6312,7 +6312,7 @@
         <v>19.29</v>
       </c>
       <c r="M80" s="1">
-        <v>21.52</v>
+        <v>22.11</v>
       </c>
       <c r="N80">
         <v>1</v>
@@ -6371,7 +6371,7 @@
         <v>54</v>
       </c>
       <c r="M81" s="1">
-        <v>60.26</v>
+        <v>61.9</v>
       </c>
       <c r="N81">
         <v>1</v>
@@ -6430,7 +6430,7 @@
         <v>13.01</v>
       </c>
       <c r="M82" s="1">
-        <v>14.51</v>
+        <v>14.91</v>
       </c>
       <c r="N82">
         <v>1</v>
@@ -6489,7 +6489,7 @@
         <v>15.7</v>
       </c>
       <c r="M83" s="1">
-        <v>17.52</v>
+        <v>17.99</v>
       </c>
       <c r="N83">
         <v>1</v>
@@ -6548,7 +6548,7 @@
         <v>17.49</v>
       </c>
       <c r="M84" s="1">
-        <v>19.52</v>
+        <v>20.05</v>
       </c>
       <c r="N84">
         <v>1</v>
@@ -6607,7 +6607,7 @@
         <v>13.9</v>
       </c>
       <c r="M85" s="1">
-        <v>15.52</v>
+        <v>15.94</v>
       </c>
       <c r="N85">
         <v>1</v>
@@ -6666,7 +6666,7 @@
         <v>17.49</v>
       </c>
       <c r="M86" s="1">
-        <v>19.52</v>
+        <v>20.05</v>
       </c>
       <c r="N86">
         <v>1</v>
@@ -6725,7 +6725,7 @@
         <v>17.49</v>
       </c>
       <c r="M87" s="1">
-        <v>19.52</v>
+        <v>20.05</v>
       </c>
       <c r="N87">
         <v>1</v>
@@ -6784,7 +6784,7 @@
         <v>19.29</v>
       </c>
       <c r="M88" s="1">
-        <v>21.52</v>
+        <v>22.11</v>
       </c>
       <c r="N88">
         <v>1</v>
@@ -6843,7 +6843,7 @@
         <v>19.29</v>
       </c>
       <c r="M89" s="1">
-        <v>21.52</v>
+        <v>22.11</v>
       </c>
       <c r="N89">
         <v>1</v>
@@ -6902,7 +6902,7 @@
         <v>14.8</v>
       </c>
       <c r="M90" s="1">
-        <v>16.52</v>
+        <v>16.97</v>
       </c>
       <c r="N90">
         <v>1</v>
@@ -6961,7 +6961,7 @@
         <v>17.94</v>
       </c>
       <c r="M91" s="1">
-        <v>20.02</v>
+        <v>20.57</v>
       </c>
       <c r="N91">
         <v>1</v>
@@ -7020,7 +7020,7 @@
         <v>19.29</v>
       </c>
       <c r="M92" s="1">
-        <v>21.52</v>
+        <v>22.11</v>
       </c>
       <c r="N92">
         <v>1</v>
@@ -7079,7 +7079,7 @@
         <v>16.15</v>
       </c>
       <c r="M93" s="1">
-        <v>18.02</v>
+        <v>18.51</v>
       </c>
       <c r="N93">
         <v>1</v>
@@ -7138,7 +7138,7 @@
         <v>16.15</v>
       </c>
       <c r="M94" s="1">
-        <v>18.02</v>
+        <v>18.51</v>
       </c>
       <c r="N94">
         <v>1</v>
@@ -7197,7 +7197,7 @@
         <v>17.94</v>
       </c>
       <c r="M95" s="1">
-        <v>20.02</v>
+        <v>20.57</v>
       </c>
       <c r="N95">
         <v>1</v>
@@ -7256,7 +7256,7 @@
         <v>16.15</v>
       </c>
       <c r="M96" s="1">
-        <v>18.02</v>
+        <v>18.51</v>
       </c>
       <c r="N96">
         <v>1</v>
@@ -7315,7 +7315,7 @@
         <v>17.94</v>
       </c>
       <c r="M97" s="1">
-        <v>20.02</v>
+        <v>20.57</v>
       </c>
       <c r="N97">
         <v>1</v>
@@ -7374,7 +7374,7 @@
         <v>8.07</v>
       </c>
       <c r="M98" s="1">
-        <v>9.01</v>
+        <v>9.25</v>
       </c>
       <c r="N98">
         <v>1</v>
@@ -7433,7 +7433,7 @@
         <v>17.49</v>
       </c>
       <c r="M99" s="1">
-        <v>19.52</v>
+        <v>20.05</v>
       </c>
       <c r="N99">
         <v>1</v>
@@ -7492,7 +7492,7 @@
         <v>17.94</v>
       </c>
       <c r="M100" s="1">
-        <v>20.02</v>
+        <v>20.57</v>
       </c>
       <c r="N100">
         <v>1</v>
@@ -7551,7 +7551,7 @@
         <v>14.8</v>
       </c>
       <c r="M101" s="1">
-        <v>16.52</v>
+        <v>16.97</v>
       </c>
       <c r="N101">
         <v>1</v>
@@ -7610,7 +7610,7 @@
         <v>9.87</v>
       </c>
       <c r="M102" s="1">
-        <v>11.01</v>
+        <v>11.31</v>
       </c>
       <c r="N102">
         <v>1</v>
@@ -7669,7 +7669,7 @@
         <v>15.25</v>
       </c>
       <c r="M103" s="1">
-        <v>17.02</v>
+        <v>17.48</v>
       </c>
       <c r="N103">
         <v>1</v>
@@ -7728,7 +7728,7 @@
         <v>17.49</v>
       </c>
       <c r="M104" s="1">
-        <v>19.52</v>
+        <v>20.05</v>
       </c>
       <c r="N104">
         <v>1</v>
@@ -7787,7 +7787,7 @@
         <v>16.15</v>
       </c>
       <c r="M105" s="1">
-        <v>18.02</v>
+        <v>18.51</v>
       </c>
       <c r="N105">
         <v>1</v>
@@ -7846,7 +7846,7 @@
         <v>10.76</v>
       </c>
       <c r="M106" s="1">
-        <v>12.01</v>
+        <v>12.34</v>
       </c>
       <c r="N106">
         <v>1</v>
@@ -7905,7 +7905,7 @@
         <v>6.28</v>
       </c>
       <c r="M107" s="1">
-        <v>7.01</v>
+        <v>7.2</v>
       </c>
       <c r="N107">
         <v>1</v>
@@ -7964,7 +7964,7 @@
         <v>17.94</v>
       </c>
       <c r="M108" s="1">
-        <v>20.02</v>
+        <v>20.57</v>
       </c>
       <c r="N108">
         <v>1</v>
@@ -8023,7 +8023,7 @@
         <v>14.8</v>
       </c>
       <c r="M109" s="1">
-        <v>16.52</v>
+        <v>16.97</v>
       </c>
       <c r="N109">
         <v>1</v>
@@ -8082,7 +8082,7 @@
         <v>14.8</v>
       </c>
       <c r="M110" s="1">
-        <v>16.52</v>
+        <v>16.97</v>
       </c>
       <c r="N110">
         <v>1</v>
@@ -8141,7 +8141,7 @@
         <v>14.8</v>
       </c>
       <c r="M111" s="1">
-        <v>16.52</v>
+        <v>16.97</v>
       </c>
       <c r="N111">
         <v>1</v>
@@ -8200,7 +8200,7 @@
         <v>15.25</v>
       </c>
       <c r="M112" s="1">
-        <v>17.02</v>
+        <v>17.48</v>
       </c>
       <c r="N112">
         <v>1</v>
@@ -8259,7 +8259,7 @@
         <v>14.8</v>
       </c>
       <c r="M113" s="1">
-        <v>16.52</v>
+        <v>16.97</v>
       </c>
       <c r="N113">
         <v>1</v>
@@ -8318,7 +8318,7 @@
         <v>17.94</v>
       </c>
       <c r="M114" s="1">
-        <v>20.02</v>
+        <v>20.57</v>
       </c>
       <c r="N114">
         <v>1</v>
@@ -8377,7 +8377,7 @@
         <v>17.94</v>
       </c>
       <c r="M115" s="1">
-        <v>20.02</v>
+        <v>20.57</v>
       </c>
       <c r="N115">
         <v>1</v>
@@ -8436,7 +8436,7 @@
         <v>17.94</v>
       </c>
       <c r="M116" s="1">
-        <v>20.02</v>
+        <v>20.57</v>
       </c>
       <c r="N116">
         <v>1</v>
@@ -8495,7 +8495,7 @@
         <v>17.94</v>
       </c>
       <c r="M117" s="1">
-        <v>20.02</v>
+        <v>20.57</v>
       </c>
       <c r="N117">
         <v>1</v>
@@ -8554,7 +8554,7 @@
         <v>13.45</v>
       </c>
       <c r="M118" s="1">
-        <v>15.02</v>
+        <v>15.42</v>
       </c>
       <c r="N118">
         <v>1</v>
@@ -8613,7 +8613,7 @@
         <v>17.94</v>
       </c>
       <c r="M119" s="1">
-        <v>20.02</v>
+        <v>20.57</v>
       </c>
       <c r="N119">
         <v>1</v>
@@ -8672,7 +8672,7 @@
         <v>17.94</v>
       </c>
       <c r="M120" s="1">
-        <v>20.02</v>
+        <v>20.57</v>
       </c>
       <c r="N120">
         <v>1</v>
@@ -8731,7 +8731,7 @@
         <v>21.53</v>
       </c>
       <c r="M121" s="1">
-        <v>24.02</v>
+        <v>24.68</v>
       </c>
       <c r="N121">
         <v>1</v>
@@ -8790,7 +8790,7 @@
         <v>17.94</v>
       </c>
       <c r="M122" s="1">
-        <v>20.02</v>
+        <v>20.57</v>
       </c>
       <c r="N122">
         <v>1</v>
@@ -8849,7 +8849,7 @@
         <v>8.97</v>
       </c>
       <c r="M123" s="1">
-        <v>10.01</v>
+        <v>10.28</v>
       </c>
       <c r="N123">
         <v>1</v>
@@ -8908,7 +8908,7 @@
         <v>13.45</v>
       </c>
       <c r="M124" s="1">
-        <v>15.02</v>
+        <v>15.42</v>
       </c>
       <c r="N124">
         <v>1</v>
@@ -8967,7 +8967,7 @@
         <v>8.97</v>
       </c>
       <c r="M125" s="1">
-        <v>10.01</v>
+        <v>10.28</v>
       </c>
       <c r="N125">
         <v>1</v>
@@ -9026,7 +9026,7 @@
         <v>14.35</v>
       </c>
       <c r="M126" s="1">
-        <v>16.02</v>
+        <v>16.45</v>
       </c>
       <c r="N126">
         <v>1</v>
@@ -9085,7 +9085,7 @@
         <v>8.97</v>
       </c>
       <c r="M127" s="1">
-        <v>10.01</v>
+        <v>10.28</v>
       </c>
       <c r="N127">
         <v>1</v>
@@ -9144,7 +9144,7 @@
         <v>19.73</v>
       </c>
       <c r="M128" s="1">
-        <v>22.02</v>
+        <v>22.62</v>
       </c>
       <c r="N128">
         <v>1</v>
@@ -9203,7 +9203,7 @@
         <v>17.94</v>
       </c>
       <c r="M129" s="1">
-        <v>20.02</v>
+        <v>20.57</v>
       </c>
       <c r="N129">
         <v>1</v>
@@ -9262,7 +9262,7 @@
         <v>14.89</v>
       </c>
       <c r="M130" s="1">
-        <v>16.62</v>
+        <v>17.07</v>
       </c>
       <c r="N130">
         <v>1</v>
@@ -9321,7 +9321,7 @@
         <v>18.63</v>
       </c>
       <c r="M131" s="1">
-        <v>20.79</v>
+        <v>21.36</v>
       </c>
       <c r="N131">
         <v>1</v>
@@ -9380,7 +9380,7 @@
         <v>19.63</v>
       </c>
       <c r="M132" s="1">
-        <v>21.9</v>
+        <v>22.5</v>
       </c>
       <c r="N132">
         <v>1</v>
@@ -9439,7 +9439,7 @@
         <v>17.25</v>
       </c>
       <c r="M133" s="1">
-        <v>19.25</v>
+        <v>19.77</v>
       </c>
       <c r="N133">
         <v>1</v>
@@ -9498,7 +9498,7 @@
         <v>19.63</v>
       </c>
       <c r="M134" s="1">
-        <v>21.9</v>
+        <v>22.5</v>
       </c>
       <c r="N134">
         <v>1</v>
@@ -9557,7 +9557,7 @@
         <v>14.89</v>
       </c>
       <c r="M135" s="1">
-        <v>16.62</v>
+        <v>17.07</v>
       </c>
       <c r="N135">
         <v>1</v>
@@ -9616,7 +9616,7 @@
         <v>18.63</v>
       </c>
       <c r="M136" s="1">
-        <v>20.79</v>
+        <v>21.36</v>
       </c>
       <c r="N136">
         <v>1</v>
@@ -9675,7 +9675,7 @@
         <v>19.63</v>
       </c>
       <c r="M137" s="1">
-        <v>21.91</v>
+        <v>22.51</v>
       </c>
       <c r="N137">
         <v>1</v>
@@ -9734,7 +9734,7 @@
         <v>14.89</v>
       </c>
       <c r="M138" s="1">
-        <v>16.62</v>
+        <v>17.07</v>
       </c>
       <c r="N138">
         <v>1</v>
@@ -9793,7 +9793,7 @@
         <v>17.25</v>
       </c>
       <c r="M139" s="1">
-        <v>19.25</v>
+        <v>19.77</v>
       </c>
       <c r="N139">
         <v>1</v>
@@ -9852,7 +9852,7 @@
         <v>19.63</v>
       </c>
       <c r="M140" s="1">
-        <v>21.9</v>
+        <v>22.5</v>
       </c>
       <c r="N140">
         <v>1</v>
@@ -9911,7 +9911,7 @@
         <v>13.8</v>
       </c>
       <c r="M141" s="1">
-        <v>15.4</v>
+        <v>15.81</v>
       </c>
       <c r="N141">
         <v>1</v>
@@ -9970,7 +9970,7 @@
         <v>8.28</v>
       </c>
       <c r="M142" s="1">
-        <v>9.24</v>
+        <v>9.49</v>
       </c>
       <c r="N142">
         <v>1</v>
@@ -10029,7 +10029,7 @@
         <v>12.42</v>
       </c>
       <c r="M143" s="1">
-        <v>13.86</v>
+        <v>14.24</v>
       </c>
       <c r="N143">
         <v>1</v>
@@ -10088,7 +10088,7 @@
         <v>20.33</v>
       </c>
       <c r="M144" s="1">
-        <v>22.68</v>
+        <v>23.3</v>
       </c>
       <c r="N144">
         <v>1</v>
@@ -10147,7 +10147,7 @@
         <v>17.25</v>
       </c>
       <c r="M145" s="1">
-        <v>19.25</v>
+        <v>19.77</v>
       </c>
       <c r="N145">
         <v>1</v>
@@ -10206,7 +10206,7 @@
         <v>18.63</v>
       </c>
       <c r="M146" s="1">
-        <v>20.79</v>
+        <v>21.36</v>
       </c>
       <c r="N146">
         <v>1</v>
@@ -10265,7 +10265,7 @@
         <v>26.57</v>
       </c>
       <c r="M147" s="1">
-        <v>29.65</v>
+        <v>30.46</v>
       </c>
       <c r="N147">
         <v>1</v>
@@ -10324,7 +10324,7 @@
         <v>29.32</v>
       </c>
       <c r="M148" s="1">
-        <v>32.72</v>
+        <v>33.61</v>
       </c>
       <c r="N148">
         <v>1</v>
@@ -10383,7 +10383,7 @@
         <v>20.7</v>
       </c>
       <c r="M149" s="1">
-        <v>23.1</v>
+        <v>23.73</v>
       </c>
       <c r="N149">
         <v>1</v>
@@ -10442,7 +10442,7 @@
         <v>19.32</v>
       </c>
       <c r="M150" s="1">
-        <v>21.56</v>
+        <v>22.15</v>
       </c>
       <c r="N150">
         <v>1</v>
@@ -10501,7 +10501,7 @@
         <v>15.18</v>
       </c>
       <c r="M151" s="1">
-        <v>16.94</v>
+        <v>17.4</v>
       </c>
       <c r="N151">
         <v>1</v>
@@ -10560,7 +10560,7 @@
         <v>13.8</v>
       </c>
       <c r="M152" s="1">
-        <v>15.4</v>
+        <v>15.81</v>
       </c>
       <c r="N152">
         <v>1</v>
@@ -10619,7 +10619,7 @@
         <v>13.8</v>
       </c>
       <c r="M153" s="1">
-        <v>15.4</v>
+        <v>15.81</v>
       </c>
       <c r="N153">
         <v>1</v>
@@ -10678,7 +10678,7 @@
         <v>13.8</v>
       </c>
       <c r="M154" s="1">
-        <v>15.4</v>
+        <v>15.81</v>
       </c>
       <c r="N154">
         <v>1</v>
@@ -10737,7 +10737,7 @@
         <v>8</v>
       </c>
       <c r="M155" s="1">
-        <v>8.93</v>
+        <v>9.17</v>
       </c>
       <c r="N155">
         <v>1</v>
@@ -10796,7 +10796,7 @@
         <v>16.56</v>
       </c>
       <c r="M156" s="1">
-        <v>18.48</v>
+        <v>18.98</v>
       </c>
       <c r="N156">
         <v>1</v>
@@ -10855,7 +10855,7 @@
         <v>9.66</v>
       </c>
       <c r="M157" s="1">
-        <v>10.78</v>
+        <v>11.07</v>
       </c>
       <c r="N157">
         <v>1</v>
@@ -10914,7 +10914,7 @@
         <v>16.56</v>
       </c>
       <c r="M158" s="1">
-        <v>18.48</v>
+        <v>18.98</v>
       </c>
       <c r="N158">
         <v>1</v>
@@ -10980,7 +10980,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>0.8496</v>
+        <v>0.9</v>
       </c>
       <c r="B5" t="s">
         <v>391</v>

</xml_diff>

<commit_message>
return category name with sql selection of product attributes as category.  this fixes category not getting displayed in pricelist output
</commit_message>
<xml_diff>
--- a/docs/masterPriceList.xlsx
+++ b/docs/masterPriceList.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="401">
   <si>
     <t>id</t>
   </si>
@@ -71,7 +71,7 @@
     <t>visible</t>
   </si>
   <si>
-    <t/>
+    <t>Pasture Raised Pork</t>
   </si>
   <si>
     <t>Baby Back Ribs</t>
@@ -124,6 +124,9 @@
     <t>1.20 - 1.50 lbs</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>Pork Chop, Boneless</t>
   </si>
   <si>
@@ -178,6 +181,9 @@
     <t>Our Pasture-Raised Pork Tenderloin from Deck Family Farm is a lean, tender cut prized for its delicate flavor and versatility. Raised on open pastures, our pigs enjoy a natural diet and humane care, resulting in exceptional meat that’s both juicy and flavorful. Whether roasted, grilled, or pan-seared, this premium cut is perfect for elegant meals or comforting weeknight dinners.</t>
   </si>
   <si>
+    <t>Fruits/Nuts Honey</t>
+  </si>
+  <si>
     <t>Raw Honey, 1 pint</t>
   </si>
   <si>
@@ -212,6 +218,9 @@
   </si>
   <si>
     <t>1/2 lb</t>
+  </si>
+  <si>
+    <t>Beef, 100% grassfed</t>
   </si>
   <si>
     <t>Bavette Steak</t>
@@ -455,6 +464,9 @@
 Instructions: Chop or grind into small pieces, simmer on low with a small amount of water, strain through a fine sieve, let fat harden in fridge. Remove the fat block from the liquid at the bottom. Cook fat to 230 degrees F to clarify.</t>
   </si>
   <si>
+    <t>Roasters &amp; Turkeys</t>
+  </si>
+  <si>
     <t>Chicken Feet, 1lb bag</t>
   </si>
   <si>
@@ -578,6 +590,9 @@
     <t>Turkey Feet are a nutrient-rich treat, perfect for making savory broths or adding depth to soups and stews. Our turkeys, including Bourbon, Bronze, and White breeds, are pasture-raised, with up to 20% of their diet consisting of fresh grass, herbs, and clover. They roam freely in fields, ensuring they are well-fed and happy. These high-quality, flavorful turkey feet are a great way to make use of every part of the bird while enjoying the natural, rich taste that comes from a diet rooted in fresh, sustainable forage.</t>
   </si>
   <si>
+    <t>Spring Lamb</t>
+  </si>
+  <si>
     <t>Ground Lamb</t>
   </si>
   <si>
@@ -669,6 +684,9 @@
   </si>
   <si>
     <t>Our Pasture-Raised Rack of Lamb from Deck Family Farm is a premium, tender cut known for its delicate flavor and elegant presentation. Raised on lush pastures, our lambs enjoy a natural diet, which results in rich, juicy meat with a clean, earthy taste. Whether roasted whole or sliced into chops, this cut is perfect for special occasions or gourmet weeknight meals.</t>
+  </si>
+  <si>
+    <t>Sausages &amp; N Free Cures</t>
   </si>
   <si>
     <t>Bacon Ends &amp; Pieces, Pork</t>
@@ -846,6 +864,9 @@
 Ingredients: Beef, Sea Salt, Brown Sugar, Sugar, Organic Dry Tamari (Organic Tamari, (Water, Organic Soybeans, Salt, Organic Alcohol) Organic Maltodextrin), Yeast, Pineapple Juice and Ascorbic Acid (Vitamin C), Dried Maple Syrup (Dextrose, Natural Maple Flavor), Black Pepper, Garlic, Onion, Cultured Celery Powder, Ginger</t>
   </si>
   <si>
+    <t>Eggs, Organic Layers</t>
+  </si>
+  <si>
     <t>Organic Pasture Raised Chicken Eggs, 1 dozen</t>
   </si>
   <si>
@@ -859,6 +880,9 @@
   </si>
   <si>
     <t>1/2 dozen</t>
+  </si>
+  <si>
+    <t>Hyland Processing</t>
   </si>
   <si>
     <t>Blueberry Maple Sausage Links</t>
@@ -994,6 +1018,9 @@
   </si>
   <si>
     <t>Our Thai Curry Sausage (Sai Ua) brings the vibrant flavors of Northern Thailand straight to your plate. Bursting with fresh aromatics like lemongrass, turmeric, lime leaf, and galangal, this sausage is like a Thai curry in every bite! A street food staple from Chiang Mai, it’s perfect served with rice, in Thai curry, or alongside grilled and pickled vegetables. Get creative by incorporating it into Asian dishes such as steam buns, dumplings, spring rolls, or a unique twist on Bánh mì.Spiciness: 6.5/10Ingredients: Pork, shallot, garlic, fish sauce (anchovies, salt, sugar), galangal, chiles, tamari (soybeans, salt, sugar), turmeric, brown cane sugar, sea salt, lemongrass, cilantro, green onion, kaffir lime leaf, shrimp paste (shrimp, salt, sugar), hog casings.Contains: Fish, shellfish, soy.</t>
+  </si>
+  <si>
+    <t>Creamy Cow Dairy</t>
   </si>
   <si>
     <t>Catalan Paprika-Rubbed Cheese, 4.2-5.2 oz</t>
@@ -1955,7 +1982,7 @@
         <v>23</v>
       </c>
       <c r="P6" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="Q6" t="s">
         <v>25</v>
@@ -1978,7 +2005,7 @@
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E7" t="s">
         <v>35</v>
@@ -2014,7 +2041,7 @@
         <v>23</v>
       </c>
       <c r="P7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Q7" t="s">
         <v>25</v>
@@ -2037,10 +2064,10 @@
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F8" s="1">
         <v>17</v>
@@ -2073,7 +2100,7 @@
         <v>23</v>
       </c>
       <c r="P8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q8" t="s">
         <v>25</v>
@@ -2096,10 +2123,10 @@
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F9" s="1">
         <v>19.5</v>
@@ -2132,7 +2159,7 @@
         <v>23</v>
       </c>
       <c r="P9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q9" t="s">
         <v>25</v>
@@ -2155,10 +2182,10 @@
         <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F10" s="1">
         <v>19.5</v>
@@ -2191,7 +2218,7 @@
         <v>23</v>
       </c>
       <c r="P10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q10" t="s">
         <v>25</v>
@@ -2208,16 +2235,16 @@
         <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F11" s="1">
         <v>12</v>
@@ -2250,7 +2277,7 @@
         <v>25</v>
       </c>
       <c r="P11" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="Q11" t="s">
         <v>25</v>
@@ -2273,10 +2300,10 @@
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F12" s="1">
         <v>14.5</v>
@@ -2309,7 +2336,7 @@
         <v>23</v>
       </c>
       <c r="P12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q12" t="s">
         <v>25</v>
@@ -2332,10 +2359,10 @@
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F13" s="1">
         <v>14.5</v>
@@ -2368,7 +2395,7 @@
         <v>23</v>
       </c>
       <c r="P13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Q13" t="s">
         <v>23</v>
@@ -2388,13 +2415,13 @@
         <v>806161</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="D14" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E14" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F14" s="1">
         <v>26</v>
@@ -2406,7 +2433,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J14" s="1">
         <v>16.9</v>
@@ -2427,7 +2454,7 @@
         <v>23</v>
       </c>
       <c r="P14" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q14" t="s">
         <v>25</v>
@@ -2447,13 +2474,13 @@
         <v>941000</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F15" s="1">
         <v>47.5</v>
@@ -2465,7 +2492,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J15" s="1">
         <v>30.88</v>
@@ -2486,7 +2513,7 @@
         <v>23</v>
       </c>
       <c r="P15" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q15" t="s">
         <v>25</v>
@@ -2506,13 +2533,13 @@
         <v>940998</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E16" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F16" s="1">
         <v>17</v>
@@ -2524,7 +2551,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J16" s="1">
         <v>11.05</v>
@@ -2545,7 +2572,7 @@
         <v>23</v>
       </c>
       <c r="P16" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q16" t="s">
         <v>25</v>
@@ -2565,13 +2592,13 @@
         <v>806159</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E17" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F17" s="1">
         <v>25</v>
@@ -2583,7 +2610,7 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J17" s="1">
         <v>16.25</v>
@@ -2604,7 +2631,7 @@
         <v>23</v>
       </c>
       <c r="P17" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="Q17" t="s">
         <v>25</v>
@@ -2624,13 +2651,13 @@
         <v>940994</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E18" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F18" s="1">
         <v>14</v>
@@ -2642,7 +2669,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J18" s="1">
         <v>9.1</v>
@@ -2663,7 +2690,7 @@
         <v>23</v>
       </c>
       <c r="P18" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="Q18" t="s">
         <v>25</v>
@@ -2683,13 +2710,13 @@
         <v>960228</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E19" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F19" s="1">
         <v>26</v>
@@ -2722,7 +2749,7 @@
         <v>23</v>
       </c>
       <c r="P19" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="Q19" t="s">
         <v>23</v>
@@ -2742,13 +2769,13 @@
         <v>813072</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D20" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E20" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F20" s="1">
         <v>16</v>
@@ -2781,7 +2808,7 @@
         <v>23</v>
       </c>
       <c r="P20" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="Q20" t="s">
         <v>23</v>
@@ -2801,10 +2828,10 @@
         <v>922135</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E21" t="s">
         <v>32</v>
@@ -2819,7 +2846,7 @@
         <v>5</v>
       </c>
       <c r="I21" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J21" s="1">
         <v>7.15</v>
@@ -2840,7 +2867,7 @@
         <v>23</v>
       </c>
       <c r="P21" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="Q21" t="s">
         <v>25</v>
@@ -2860,13 +2887,13 @@
         <v>813075</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E22" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F22" s="1">
         <v>26</v>
@@ -2899,7 +2926,7 @@
         <v>23</v>
       </c>
       <c r="P22" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="Q22" t="s">
         <v>25</v>
@@ -2919,13 +2946,13 @@
         <v>805660</v>
       </c>
       <c r="C23" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D23" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E23" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F23" s="1">
         <v>9.5</v>
@@ -2958,7 +2985,7 @@
         <v>23</v>
       </c>
       <c r="P23" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="Q23" t="s">
         <v>23</v>
@@ -2978,13 +3005,13 @@
         <v>825832</v>
       </c>
       <c r="C24" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D24" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E24" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F24" s="1">
         <v>26</v>
@@ -3017,7 +3044,7 @@
         <v>23</v>
       </c>
       <c r="P24" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="Q24" t="s">
         <v>25</v>
@@ -3037,13 +3064,13 @@
         <v>841579</v>
       </c>
       <c r="C25" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D25" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E25" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F25" s="1">
         <v>26</v>
@@ -3076,7 +3103,7 @@
         <v>23</v>
       </c>
       <c r="P25" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="Q25" t="s">
         <v>25</v>
@@ -3096,10 +3123,10 @@
         <v>825834</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D26" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E26" t="s">
         <v>32</v>
@@ -3114,7 +3141,7 @@
         <v>3.5</v>
       </c>
       <c r="I26" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J26" s="1">
         <v>9.75</v>
@@ -3135,7 +3162,7 @@
         <v>23</v>
       </c>
       <c r="P26" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="Q26" t="s">
         <v>23</v>
@@ -3155,13 +3182,13 @@
         <v>813076</v>
       </c>
       <c r="C27" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D27" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E27" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F27" s="1">
         <v>13</v>
@@ -3194,7 +3221,7 @@
         <v>23</v>
       </c>
       <c r="P27" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="Q27" t="s">
         <v>25</v>
@@ -3214,13 +3241,13 @@
         <v>813071</v>
       </c>
       <c r="C28" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D28" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E28" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F28" s="1">
         <v>19.5</v>
@@ -3253,7 +3280,7 @@
         <v>23</v>
       </c>
       <c r="P28" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="Q28" t="s">
         <v>25</v>
@@ -3273,13 +3300,13 @@
         <v>894281</v>
       </c>
       <c r="C29" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D29" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E29" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F29" s="1">
         <v>19.5</v>
@@ -3312,7 +3339,7 @@
         <v>23</v>
       </c>
       <c r="P29" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="Q29" t="s">
         <v>25</v>
@@ -3329,16 +3356,16 @@
         <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C30" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D30" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E30" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F30" s="1">
         <v>10.5</v>
@@ -3371,7 +3398,7 @@
         <v>25</v>
       </c>
       <c r="P30" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="Q30" t="s">
         <v>25</v>
@@ -3391,13 +3418,13 @@
         <v>805667</v>
       </c>
       <c r="C31" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D31" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E31" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F31" s="1">
         <v>18.5</v>
@@ -3430,7 +3457,7 @@
         <v>23</v>
       </c>
       <c r="P31" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="Q31" t="s">
         <v>23</v>
@@ -3450,13 +3477,13 @@
         <v>813067</v>
       </c>
       <c r="C32" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D32" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E32" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F32" s="1">
         <v>43</v>
@@ -3489,7 +3516,7 @@
         <v>23</v>
       </c>
       <c r="P32" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="Q32" t="s">
         <v>25</v>
@@ -3509,13 +3536,13 @@
         <v>825833</v>
       </c>
       <c r="C33" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D33" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E33" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="F33" s="1">
         <v>9.5</v>
@@ -3548,7 +3575,7 @@
         <v>23</v>
       </c>
       <c r="P33" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="Q33" t="s">
         <v>23</v>
@@ -3568,13 +3595,13 @@
         <v>869027</v>
       </c>
       <c r="C34" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D34" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E34" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F34" s="1">
         <v>21</v>
@@ -3607,7 +3634,7 @@
         <v>23</v>
       </c>
       <c r="P34" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="Q34" t="s">
         <v>25</v>
@@ -3627,13 +3654,13 @@
         <v>856878</v>
       </c>
       <c r="C35" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D35" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E35" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="F35" s="1">
         <v>16</v>
@@ -3666,7 +3693,7 @@
         <v>23</v>
       </c>
       <c r="P35" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="Q35" t="s">
         <v>25</v>
@@ -3686,13 +3713,13 @@
         <v>941001</v>
       </c>
       <c r="C36" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D36" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E36" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F36" s="1">
         <v>17</v>
@@ -3725,7 +3752,7 @@
         <v>23</v>
       </c>
       <c r="P36" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="Q36" t="s">
         <v>23</v>
@@ -3745,13 +3772,13 @@
         <v>941002</v>
       </c>
       <c r="C37" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D37" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E37" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F37" s="1">
         <v>18</v>
@@ -3784,7 +3811,7 @@
         <v>23</v>
       </c>
       <c r="P37" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="Q37" t="s">
         <v>25</v>
@@ -3804,13 +3831,13 @@
         <v>805658</v>
       </c>
       <c r="C38" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D38" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E38" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="F38" s="1">
         <v>16</v>
@@ -3843,7 +3870,7 @@
         <v>23</v>
       </c>
       <c r="P38" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="Q38" t="s">
         <v>23</v>
@@ -3863,13 +3890,13 @@
         <v>813074</v>
       </c>
       <c r="C39" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D39" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E39" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F39" s="1">
         <v>26</v>
@@ -3902,7 +3929,7 @@
         <v>23</v>
       </c>
       <c r="P39" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="Q39" t="s">
         <v>25</v>
@@ -3922,10 +3949,10 @@
         <v>805664</v>
       </c>
       <c r="C40" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D40" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E40" t="s">
         <v>27</v>
@@ -3961,7 +3988,7 @@
         <v>23</v>
       </c>
       <c r="P40" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="Q40" t="s">
         <v>25</v>
@@ -3981,13 +4008,13 @@
         <v>825830</v>
       </c>
       <c r="C41" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D41" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="E41" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F41" s="1">
         <v>26</v>
@@ -4020,7 +4047,7 @@
         <v>23</v>
       </c>
       <c r="P41" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="Q41" t="s">
         <v>25</v>
@@ -4040,13 +4067,13 @@
         <v>805701</v>
       </c>
       <c r="C42" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D42" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="E42" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="F42" s="1">
         <v>19.5</v>
@@ -4079,7 +4106,7 @@
         <v>23</v>
       </c>
       <c r="P42" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="Q42" t="s">
         <v>23</v>
@@ -4099,13 +4126,13 @@
         <v>805688</v>
       </c>
       <c r="C43" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D43" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="E43" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F43" s="1">
         <v>12</v>
@@ -4138,7 +4165,7 @@
         <v>23</v>
       </c>
       <c r="P43" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="Q43" t="s">
         <v>25</v>
@@ -4158,13 +4185,13 @@
         <v>805716</v>
       </c>
       <c r="C44" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D44" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="E44" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="F44" s="1">
         <v>37</v>
@@ -4197,7 +4224,7 @@
         <v>23</v>
       </c>
       <c r="P44" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="Q44" t="s">
         <v>25</v>
@@ -4217,13 +4244,13 @@
         <v>805689</v>
       </c>
       <c r="C45" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D45" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E45" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F45" s="1">
         <v>12</v>
@@ -4256,7 +4283,7 @@
         <v>23</v>
       </c>
       <c r="P45" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="Q45" t="s">
         <v>25</v>
@@ -4276,13 +4303,13 @@
         <v>805668</v>
       </c>
       <c r="C46" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D46" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="E46" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="F46" s="1">
         <v>40.5</v>
@@ -4315,7 +4342,7 @@
         <v>23</v>
       </c>
       <c r="P46" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="Q46" t="s">
         <v>23</v>
@@ -4335,13 +4362,13 @@
         <v>929452</v>
       </c>
       <c r="C47" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D47" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E47" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F47" s="1">
         <v>26</v>
@@ -4374,7 +4401,7 @@
         <v>23</v>
       </c>
       <c r="P47" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="Q47" t="s">
         <v>25</v>
@@ -4394,13 +4421,13 @@
         <v>894282</v>
       </c>
       <c r="C48" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D48" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E48" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="F48" s="1">
         <v>26</v>
@@ -4433,7 +4460,7 @@
         <v>23</v>
       </c>
       <c r="P48" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="Q48" t="s">
         <v>25</v>
@@ -4453,13 +4480,13 @@
         <v>813069</v>
       </c>
       <c r="C49" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D49" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="E49" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F49" s="1">
         <v>26</v>
@@ -4492,7 +4519,7 @@
         <v>23</v>
       </c>
       <c r="P49" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="Q49" t="s">
         <v>25</v>
@@ -4512,13 +4539,13 @@
         <v>814845</v>
       </c>
       <c r="C50" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D50" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="E50" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="F50" s="1">
         <v>25</v>
@@ -4551,7 +4578,7 @@
         <v>23</v>
       </c>
       <c r="P50" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="Q50" t="s">
         <v>23</v>
@@ -4571,13 +4598,13 @@
         <v>883799</v>
       </c>
       <c r="C51" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="D51" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E51" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="F51" s="1">
         <v>5</v>
@@ -4610,7 +4637,7 @@
         <v>23</v>
       </c>
       <c r="P51" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="Q51" t="s">
         <v>25</v>
@@ -4630,13 +4657,13 @@
         <v>813079</v>
       </c>
       <c r="C52" t="s">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="D52" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="E52" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="F52" s="1">
         <v>9.5</v>
@@ -4648,7 +4675,7 @@
         <v>1</v>
       </c>
       <c r="I52" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J52" s="1">
         <v>6.17</v>
@@ -4669,7 +4696,7 @@
         <v>23</v>
       </c>
       <c r="P52" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="Q52" t="s">
         <v>25</v>
@@ -4689,13 +4716,13 @@
         <v>818957</v>
       </c>
       <c r="C53" t="s">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="D53" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="E53" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="F53" s="1">
         <v>9.5</v>
@@ -4707,7 +4734,7 @@
         <v>0.5</v>
       </c>
       <c r="I53" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J53" s="1">
         <v>6.17</v>
@@ -4728,7 +4755,7 @@
         <v>23</v>
       </c>
       <c r="P53" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="Q53" t="s">
         <v>25</v>
@@ -4748,13 +4775,13 @@
         <v>805677</v>
       </c>
       <c r="C54" t="s">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="D54" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="E54" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="F54" s="1">
         <v>12</v>
@@ -4766,7 +4793,7 @@
         <v>0.5</v>
       </c>
       <c r="I54" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J54" s="1">
         <v>7.8</v>
@@ -4787,7 +4814,7 @@
         <v>23</v>
       </c>
       <c r="P54" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="Q54" t="s">
         <v>25</v>
@@ -4807,13 +4834,13 @@
         <v>805669</v>
       </c>
       <c r="C55" t="s">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="D55" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="E55" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="F55" s="1">
         <v>18</v>
@@ -4846,7 +4873,7 @@
         <v>23</v>
       </c>
       <c r="P55" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="Q55" t="s">
         <v>25</v>
@@ -4866,13 +4893,13 @@
         <v>900315</v>
       </c>
       <c r="C56" t="s">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="D56" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="E56" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="F56" s="1">
         <v>18.5</v>
@@ -4905,7 +4932,7 @@
         <v>25</v>
       </c>
       <c r="P56" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="Q56" t="s">
         <v>25</v>
@@ -4925,13 +4952,13 @@
         <v>805676</v>
       </c>
       <c r="C57" t="s">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="D57" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="E57" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="F57" s="1">
         <v>15.5</v>
@@ -4964,7 +4991,7 @@
         <v>23</v>
       </c>
       <c r="P57" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="Q57" t="s">
         <v>25</v>
@@ -4984,13 +5011,13 @@
         <v>805679</v>
       </c>
       <c r="C58" t="s">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="D58" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E58" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="F58" s="1">
         <v>12</v>
@@ -5023,7 +5050,7 @@
         <v>23</v>
       </c>
       <c r="P58" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="Q58" t="s">
         <v>25</v>
@@ -5043,13 +5070,13 @@
         <v>805673</v>
       </c>
       <c r="C59" t="s">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="D59" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="E59" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F59" s="1">
         <v>9</v>
@@ -5082,7 +5109,7 @@
         <v>23</v>
       </c>
       <c r="P59" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="Q59" t="s">
         <v>25</v>
@@ -5102,13 +5129,13 @@
         <v>953035</v>
       </c>
       <c r="C60" t="s">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="D60" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="E60" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="F60" s="1">
         <v>9.5</v>
@@ -5141,7 +5168,7 @@
         <v>23</v>
       </c>
       <c r="P60" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="Q60" t="s">
         <v>25</v>
@@ -5161,13 +5188,13 @@
         <v>953036</v>
       </c>
       <c r="C61" t="s">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="D61" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="E61" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="F61" s="1">
         <v>10</v>
@@ -5200,7 +5227,7 @@
         <v>23</v>
       </c>
       <c r="P61" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="Q61" t="s">
         <v>25</v>
@@ -5220,13 +5247,13 @@
         <v>953039</v>
       </c>
       <c r="C62" t="s">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="D62" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="E62" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="F62" s="1">
         <v>10.5</v>
@@ -5259,7 +5286,7 @@
         <v>23</v>
       </c>
       <c r="P62" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="Q62" t="s">
         <v>25</v>
@@ -5276,16 +5303,16 @@
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C63" t="s">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="D63" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="E63" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="F63" s="1">
         <v>12</v>
@@ -5318,7 +5345,7 @@
         <v>25</v>
       </c>
       <c r="P63" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="Q63" t="s">
         <v>25</v>
@@ -5335,16 +5362,16 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C64" t="s">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="D64" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E64" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="F64" s="1">
         <v>12</v>
@@ -5377,7 +5404,7 @@
         <v>25</v>
       </c>
       <c r="P64" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="Q64" t="s">
         <v>25</v>
@@ -5397,13 +5424,13 @@
         <v>805661</v>
       </c>
       <c r="C65" t="s">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="D65" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="E65" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="F65" s="1">
         <v>12</v>
@@ -5436,7 +5463,7 @@
         <v>23</v>
       </c>
       <c r="P65" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="Q65" t="s">
         <v>25</v>
@@ -5456,13 +5483,13 @@
         <v>805685</v>
       </c>
       <c r="C66" t="s">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="D66" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="E66" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F66" s="1">
         <v>18.5</v>
@@ -5474,7 +5501,7 @@
         <v>3.8</v>
       </c>
       <c r="I66" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J66" s="1">
         <v>12.03</v>
@@ -5495,7 +5522,7 @@
         <v>23</v>
       </c>
       <c r="P66" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="Q66" t="s">
         <v>25</v>
@@ -5515,13 +5542,13 @@
         <v>814849</v>
       </c>
       <c r="C67" t="s">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="D67" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E67" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="F67" s="1">
         <v>12</v>
@@ -5533,7 +5560,7 @@
         <v>2</v>
       </c>
       <c r="I67" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J67" s="1">
         <v>7.8</v>
@@ -5554,7 +5581,7 @@
         <v>23</v>
       </c>
       <c r="P67" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="Q67" t="s">
         <v>25</v>
@@ -5574,10 +5601,10 @@
         <v>813092</v>
       </c>
       <c r="C68" t="s">
-        <v>19</v>
+        <v>191</v>
       </c>
       <c r="D68" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="E68" t="s">
         <v>27</v>
@@ -5613,7 +5640,7 @@
         <v>23</v>
       </c>
       <c r="P68" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="Q68" t="s">
         <v>25</v>
@@ -5633,10 +5660,10 @@
         <v>825835</v>
       </c>
       <c r="C69" t="s">
-        <v>19</v>
+        <v>191</v>
       </c>
       <c r="D69" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="E69" t="s">
         <v>32</v>
@@ -5672,7 +5699,7 @@
         <v>23</v>
       </c>
       <c r="P69" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="Q69" t="s">
         <v>25</v>
@@ -5692,13 +5719,13 @@
         <v>922133</v>
       </c>
       <c r="C70" t="s">
-        <v>19</v>
+        <v>191</v>
       </c>
       <c r="D70" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="E70" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="F70" s="1">
         <v>24</v>
@@ -5731,7 +5758,7 @@
         <v>23</v>
       </c>
       <c r="P70" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="Q70" t="s">
         <v>25</v>
@@ -5751,13 +5778,13 @@
         <v>913064</v>
       </c>
       <c r="C71" t="s">
-        <v>19</v>
+        <v>191</v>
       </c>
       <c r="D71" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="E71" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="F71" s="1">
         <v>24</v>
@@ -5790,7 +5817,7 @@
         <v>23</v>
       </c>
       <c r="P71" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="Q71" t="s">
         <v>25</v>
@@ -5810,13 +5837,13 @@
         <v>939774</v>
       </c>
       <c r="C72" t="s">
-        <v>19</v>
+        <v>191</v>
       </c>
       <c r="D72" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="E72" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="F72" s="1">
         <v>9.5</v>
@@ -5849,7 +5876,7 @@
         <v>23</v>
       </c>
       <c r="P72" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="Q72" t="s">
         <v>23</v>
@@ -5869,13 +5896,13 @@
         <v>825839</v>
       </c>
       <c r="C73" t="s">
-        <v>19</v>
+        <v>191</v>
       </c>
       <c r="D73" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="E73" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="F73" s="1">
         <v>21.5</v>
@@ -5908,7 +5935,7 @@
         <v>23</v>
       </c>
       <c r="P73" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="Q73" t="s">
         <v>23</v>
@@ -5928,13 +5955,13 @@
         <v>805703</v>
       </c>
       <c r="C74" t="s">
-        <v>19</v>
+        <v>191</v>
       </c>
       <c r="D74" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="E74" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="F74" s="1">
         <v>15.5</v>
@@ -5967,7 +5994,7 @@
         <v>23</v>
       </c>
       <c r="P74" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="Q74" t="s">
         <v>25</v>
@@ -5987,13 +6014,13 @@
         <v>805705</v>
       </c>
       <c r="C75" t="s">
-        <v>19</v>
+        <v>191</v>
       </c>
       <c r="D75" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="E75" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F75" s="1">
         <v>18.5</v>
@@ -6026,7 +6053,7 @@
         <v>23</v>
       </c>
       <c r="P75" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="Q75" t="s">
         <v>25</v>
@@ -6046,13 +6073,13 @@
         <v>825840</v>
       </c>
       <c r="C76" t="s">
-        <v>19</v>
+        <v>191</v>
       </c>
       <c r="D76" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="E76" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F76" s="1">
         <v>19</v>
@@ -6085,7 +6112,7 @@
         <v>23</v>
       </c>
       <c r="P76" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="Q76" t="s">
         <v>25</v>
@@ -6105,13 +6132,13 @@
         <v>805710</v>
       </c>
       <c r="C77" t="s">
-        <v>19</v>
+        <v>191</v>
       </c>
       <c r="D77" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="E77" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="F77" s="1">
         <v>19</v>
@@ -6144,7 +6171,7 @@
         <v>23</v>
       </c>
       <c r="P77" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="Q77" t="s">
         <v>25</v>
@@ -6164,13 +6191,13 @@
         <v>805711</v>
       </c>
       <c r="C78" t="s">
-        <v>19</v>
+        <v>191</v>
       </c>
       <c r="D78" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="E78" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="F78" s="1">
         <v>20</v>
@@ -6203,7 +6230,7 @@
         <v>23</v>
       </c>
       <c r="P78" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="Q78" t="s">
         <v>25</v>
@@ -6220,16 +6247,16 @@
         <v>65</v>
       </c>
       <c r="B79" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C79" t="s">
-        <v>19</v>
+        <v>191</v>
       </c>
       <c r="D79" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="E79" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F79" s="1">
         <v>13</v>
@@ -6262,7 +6289,7 @@
         <v>25</v>
       </c>
       <c r="P79" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="Q79" t="s">
         <v>25</v>
@@ -6282,13 +6309,13 @@
         <v>805712</v>
       </c>
       <c r="C80" t="s">
-        <v>19</v>
+        <v>191</v>
       </c>
       <c r="D80" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="E80" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F80" s="1">
         <v>21.5</v>
@@ -6321,7 +6348,7 @@
         <v>23</v>
       </c>
       <c r="P80" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="Q80" t="s">
         <v>25</v>
@@ -6341,13 +6368,13 @@
         <v>805659</v>
       </c>
       <c r="C81" t="s">
-        <v>19</v>
+        <v>191</v>
       </c>
       <c r="D81" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="E81" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="F81" s="1">
         <v>21.5</v>
@@ -6380,7 +6407,7 @@
         <v>23</v>
       </c>
       <c r="P81" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="Q81" t="s">
         <v>25</v>
@@ -6400,13 +6427,13 @@
         <v>805653</v>
       </c>
       <c r="C82" t="s">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="D82" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="E82" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="F82" s="1">
         <v>14.5</v>
@@ -6418,7 +6445,7 @@
         <v>0</v>
       </c>
       <c r="I82" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J82" s="1">
         <v>9.43</v>
@@ -6439,7 +6466,7 @@
         <v>23</v>
       </c>
       <c r="P82" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="Q82" t="s">
         <v>25</v>
@@ -6459,13 +6486,13 @@
         <v>805724</v>
       </c>
       <c r="C83" t="s">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="D83" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="E83" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="F83" s="1">
         <v>17.5</v>
@@ -6477,7 +6504,7 @@
         <v>0</v>
       </c>
       <c r="I83" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J83" s="1">
         <v>11.38</v>
@@ -6498,7 +6525,7 @@
         <v>23</v>
       </c>
       <c r="P83" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="Q83" t="s">
         <v>25</v>
@@ -6518,13 +6545,13 @@
         <v>813084</v>
       </c>
       <c r="C84" t="s">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="D84" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="E84" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="F84" s="1">
         <v>19.5</v>
@@ -6536,7 +6563,7 @@
         <v>0</v>
       </c>
       <c r="I84" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J84" s="1">
         <v>12.68</v>
@@ -6557,7 +6584,7 @@
         <v>23</v>
       </c>
       <c r="P84" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="Q84" t="s">
         <v>25</v>
@@ -6577,13 +6604,13 @@
         <v>813086</v>
       </c>
       <c r="C85" t="s">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="D85" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="E85" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="F85" s="1">
         <v>15.5</v>
@@ -6595,7 +6622,7 @@
         <v>0</v>
       </c>
       <c r="I85" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J85" s="1">
         <v>10.08</v>
@@ -6616,7 +6643,7 @@
         <v>23</v>
       </c>
       <c r="P85" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="Q85" t="s">
         <v>25</v>
@@ -6636,13 +6663,13 @@
         <v>805686</v>
       </c>
       <c r="C86" t="s">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="D86" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="E86" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="F86" s="1">
         <v>19.5</v>
@@ -6654,7 +6681,7 @@
         <v>0</v>
       </c>
       <c r="I86" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J86" s="1">
         <v>12.68</v>
@@ -6675,7 +6702,7 @@
         <v>23</v>
       </c>
       <c r="P86" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="Q86" t="s">
         <v>25</v>
@@ -6695,13 +6722,13 @@
         <v>805693</v>
       </c>
       <c r="C87" t="s">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="D87" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E87" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="F87" s="1">
         <v>19.5</v>
@@ -6713,7 +6740,7 @@
         <v>0</v>
       </c>
       <c r="I87" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J87" s="1">
         <v>12.68</v>
@@ -6734,7 +6761,7 @@
         <v>23</v>
       </c>
       <c r="P87" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="Q87" t="s">
         <v>25</v>
@@ -6754,13 +6781,13 @@
         <v>882704</v>
       </c>
       <c r="C88" t="s">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="D88" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="E88" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="F88" s="1">
         <v>21.5</v>
@@ -6772,7 +6799,7 @@
         <v>0</v>
       </c>
       <c r="I88" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J88" s="1">
         <v>13.97</v>
@@ -6793,7 +6820,7 @@
         <v>23</v>
       </c>
       <c r="P88" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="Q88" t="s">
         <v>25</v>
@@ -6813,13 +6840,13 @@
         <v>963826</v>
       </c>
       <c r="C89" t="s">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="D89" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="E89" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="F89" s="1">
         <v>21.5</v>
@@ -6831,7 +6858,7 @@
         <v>0</v>
       </c>
       <c r="I89" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J89" s="1">
         <v>13.97</v>
@@ -6852,7 +6879,7 @@
         <v>25</v>
       </c>
       <c r="P89" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="Q89" t="s">
         <v>25</v>
@@ -6872,13 +6899,13 @@
         <v>805713</v>
       </c>
       <c r="C90" t="s">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="D90" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="E90" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="F90" s="1">
         <v>16.5</v>
@@ -6890,7 +6917,7 @@
         <v>0</v>
       </c>
       <c r="I90" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J90" s="1">
         <v>10.72</v>
@@ -6911,7 +6938,7 @@
         <v>23</v>
       </c>
       <c r="P90" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="Q90" t="s">
         <v>25</v>
@@ -6931,13 +6958,13 @@
         <v>827440</v>
       </c>
       <c r="C91" t="s">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="D91" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="E91" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="F91" s="1">
         <v>20</v>
@@ -6949,7 +6976,7 @@
         <v>0</v>
       </c>
       <c r="I91" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J91" s="1">
         <v>13</v>
@@ -6970,7 +6997,7 @@
         <v>23</v>
       </c>
       <c r="P91" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="Q91" t="s">
         <v>25</v>
@@ -6990,13 +7017,13 @@
         <v>901753</v>
       </c>
       <c r="C92" t="s">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="D92" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="E92" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="F92" s="1">
         <v>21.5</v>
@@ -7008,7 +7035,7 @@
         <v>0</v>
       </c>
       <c r="I92" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J92" s="1">
         <v>13.97</v>
@@ -7029,7 +7056,7 @@
         <v>23</v>
       </c>
       <c r="P92" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="Q92" t="s">
         <v>25</v>
@@ -7049,13 +7076,13 @@
         <v>859028</v>
       </c>
       <c r="C93" t="s">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="D93" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="E93" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="F93" s="1">
         <v>18</v>
@@ -7067,7 +7094,7 @@
         <v>0</v>
       </c>
       <c r="I93" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J93" s="1">
         <v>11.7</v>
@@ -7088,7 +7115,7 @@
         <v>23</v>
       </c>
       <c r="P93" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="Q93" t="s">
         <v>25</v>
@@ -7108,13 +7135,13 @@
         <v>805675</v>
       </c>
       <c r="C94" t="s">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="D94" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="E94" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="F94" s="1">
         <v>18</v>
@@ -7126,7 +7153,7 @@
         <v>0</v>
       </c>
       <c r="I94" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J94" s="1">
         <v>11.7</v>
@@ -7147,7 +7174,7 @@
         <v>23</v>
       </c>
       <c r="P94" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="Q94" t="s">
         <v>25</v>
@@ -7167,13 +7194,13 @@
         <v>805719</v>
       </c>
       <c r="C95" t="s">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="D95" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="E95" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="F95" s="1">
         <v>20</v>
@@ -7185,7 +7212,7 @@
         <v>0</v>
       </c>
       <c r="I95" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J95" s="1">
         <v>13</v>
@@ -7206,7 +7233,7 @@
         <v>23</v>
       </c>
       <c r="P95" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="Q95" t="s">
         <v>25</v>
@@ -7226,13 +7253,13 @@
         <v>805720</v>
       </c>
       <c r="C96" t="s">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="D96" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="E96" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="F96" s="1">
         <v>18</v>
@@ -7244,7 +7271,7 @@
         <v>0</v>
       </c>
       <c r="I96" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J96" s="1">
         <v>11.7</v>
@@ -7265,7 +7292,7 @@
         <v>23</v>
       </c>
       <c r="P96" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="Q96" t="s">
         <v>25</v>
@@ -7285,13 +7312,13 @@
         <v>805721</v>
       </c>
       <c r="C97" t="s">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="D97" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="E97" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="F97" s="1">
         <v>20</v>
@@ -7303,7 +7330,7 @@
         <v>6</v>
       </c>
       <c r="I97" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J97" s="1">
         <v>13</v>
@@ -7324,7 +7351,7 @@
         <v>23</v>
       </c>
       <c r="P97" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="Q97" t="s">
         <v>25</v>
@@ -7344,13 +7371,13 @@
         <v>858286</v>
       </c>
       <c r="C98" t="s">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="D98" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="E98" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="F98" s="1">
         <v>9</v>
@@ -7362,7 +7389,7 @@
         <v>0</v>
       </c>
       <c r="I98" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J98" s="1">
         <v>5.85</v>
@@ -7383,7 +7410,7 @@
         <v>23</v>
       </c>
       <c r="P98" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="Q98" t="s">
         <v>25</v>
@@ -7403,13 +7430,13 @@
         <v>805682</v>
       </c>
       <c r="C99" t="s">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="D99" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="E99" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="F99" s="1">
         <v>19.5</v>
@@ -7421,7 +7448,7 @@
         <v>0</v>
       </c>
       <c r="I99" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J99" s="1">
         <v>12.68</v>
@@ -7442,7 +7469,7 @@
         <v>23</v>
       </c>
       <c r="P99" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="Q99" t="s">
         <v>25</v>
@@ -7462,13 +7489,13 @@
         <v>805670</v>
       </c>
       <c r="C100" t="s">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="D100" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="E100" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="F100" s="1">
         <v>20</v>
@@ -7480,7 +7507,7 @@
         <v>0</v>
       </c>
       <c r="I100" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J100" s="1">
         <v>13</v>
@@ -7501,7 +7528,7 @@
         <v>23</v>
       </c>
       <c r="P100" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="Q100" t="s">
         <v>25</v>
@@ -7521,13 +7548,13 @@
         <v>805678</v>
       </c>
       <c r="C101" t="s">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="D101" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="E101" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="F101" s="1">
         <v>16.5</v>
@@ -7539,7 +7566,7 @@
         <v>0</v>
       </c>
       <c r="I101" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J101" s="1">
         <v>10.72</v>
@@ -7560,7 +7587,7 @@
         <v>23</v>
       </c>
       <c r="P101" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="Q101" t="s">
         <v>25</v>
@@ -7580,13 +7607,13 @@
         <v>940154</v>
       </c>
       <c r="C102" t="s">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="D102" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="E102" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="F102" s="1">
         <v>11</v>
@@ -7598,7 +7625,7 @@
         <v>0.5</v>
       </c>
       <c r="I102" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J102" s="1">
         <v>7.15</v>
@@ -7619,7 +7646,7 @@
         <v>23</v>
       </c>
       <c r="P102" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="Q102" t="s">
         <v>25</v>
@@ -7639,13 +7666,13 @@
         <v>805687</v>
       </c>
       <c r="C103" t="s">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="D103" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="E103" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="F103" s="1">
         <v>17</v>
@@ -7657,7 +7684,7 @@
         <v>0</v>
       </c>
       <c r="I103" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J103" s="1">
         <v>11.05</v>
@@ -7678,7 +7705,7 @@
         <v>23</v>
       </c>
       <c r="P103" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="Q103" t="s">
         <v>25</v>
@@ -7698,13 +7725,13 @@
         <v>805692</v>
       </c>
       <c r="C104" t="s">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="D104" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="E104" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="F104" s="1">
         <v>19.5</v>
@@ -7716,7 +7743,7 @@
         <v>0</v>
       </c>
       <c r="I104" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J104" s="1">
         <v>12.68</v>
@@ -7737,7 +7764,7 @@
         <v>23</v>
       </c>
       <c r="P104" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="Q104" t="s">
         <v>25</v>
@@ -7757,13 +7784,13 @@
         <v>805694</v>
       </c>
       <c r="C105" t="s">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="D105" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="E105" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="F105" s="1">
         <v>18</v>
@@ -7775,7 +7802,7 @@
         <v>0</v>
       </c>
       <c r="I105" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J105" s="1">
         <v>11.7</v>
@@ -7796,7 +7823,7 @@
         <v>23</v>
       </c>
       <c r="P105" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="Q105" t="s">
         <v>25</v>
@@ -7816,13 +7843,13 @@
         <v>941005</v>
       </c>
       <c r="C106" t="s">
-        <v>19</v>
+        <v>278</v>
       </c>
       <c r="D106" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="E106" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="F106" s="1">
         <v>12</v>
@@ -7834,7 +7861,7 @@
         <v>1</v>
       </c>
       <c r="I106" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J106" s="1">
         <v>7.8</v>
@@ -7855,7 +7882,7 @@
         <v>23</v>
       </c>
       <c r="P106" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="Q106" t="s">
         <v>25</v>
@@ -7875,13 +7902,13 @@
         <v>805459</v>
       </c>
       <c r="C107" t="s">
-        <v>19</v>
+        <v>278</v>
       </c>
       <c r="D107" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="E107" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="F107" s="1">
         <v>7</v>
@@ -7893,7 +7920,7 @@
         <v>0.5</v>
       </c>
       <c r="I107" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J107" s="1">
         <v>4.55</v>
@@ -7914,7 +7941,7 @@
         <v>23</v>
       </c>
       <c r="P107" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="Q107" t="s">
         <v>25</v>
@@ -7934,13 +7961,13 @@
         <v>900311</v>
       </c>
       <c r="C108" t="s">
-        <v>19</v>
+        <v>284</v>
       </c>
       <c r="D108" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="E108" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="F108" s="1">
         <v>20</v>
@@ -7952,7 +7979,7 @@
         <v>14</v>
       </c>
       <c r="I108" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J108" s="1">
         <v>13</v>
@@ -7973,7 +8000,7 @@
         <v>23</v>
       </c>
       <c r="P108" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="Q108" t="s">
         <v>25</v>
@@ -7993,13 +8020,13 @@
         <v>840848</v>
       </c>
       <c r="C109" t="s">
-        <v>19</v>
+        <v>284</v>
       </c>
       <c r="D109" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="E109" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="F109" s="1">
         <v>16.5</v>
@@ -8011,7 +8038,7 @@
         <v>12</v>
       </c>
       <c r="I109" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J109" s="1">
         <v>10.72</v>
@@ -8032,7 +8059,7 @@
         <v>23</v>
       </c>
       <c r="P109" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="Q109" t="s">
         <v>25</v>
@@ -8052,13 +8079,13 @@
         <v>840823</v>
       </c>
       <c r="C110" t="s">
-        <v>19</v>
+        <v>284</v>
       </c>
       <c r="D110" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="E110" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="F110" s="1">
         <v>16.5</v>
@@ -8070,7 +8097,7 @@
         <v>12</v>
       </c>
       <c r="I110" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J110" s="1">
         <v>10.72</v>
@@ -8091,7 +8118,7 @@
         <v>23</v>
       </c>
       <c r="P110" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="Q110" t="s">
         <v>25</v>
@@ -8111,13 +8138,13 @@
         <v>913652</v>
       </c>
       <c r="C111" t="s">
-        <v>19</v>
+        <v>284</v>
       </c>
       <c r="D111" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="E111" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="F111" s="1">
         <v>16.5</v>
@@ -8129,7 +8156,7 @@
         <v>12</v>
       </c>
       <c r="I111" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J111" s="1">
         <v>10.72</v>
@@ -8150,7 +8177,7 @@
         <v>23</v>
       </c>
       <c r="P111" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="Q111" t="s">
         <v>25</v>
@@ -8170,13 +8197,13 @@
         <v>805696</v>
       </c>
       <c r="C112" t="s">
-        <v>19</v>
+        <v>284</v>
       </c>
       <c r="D112" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="E112" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="F112" s="1">
         <v>17</v>
@@ -8188,7 +8215,7 @@
         <v>14</v>
       </c>
       <c r="I112" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J112" s="1">
         <v>11.05</v>
@@ -8209,7 +8236,7 @@
         <v>23</v>
       </c>
       <c r="P112" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="Q112" t="s">
         <v>25</v>
@@ -8229,13 +8256,13 @@
         <v>913651</v>
       </c>
       <c r="C113" t="s">
-        <v>19</v>
+        <v>284</v>
       </c>
       <c r="D113" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
       <c r="E113" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="F113" s="1">
         <v>16.5</v>
@@ -8247,7 +8274,7 @@
         <v>12</v>
       </c>
       <c r="I113" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J113" s="1">
         <v>10.72</v>
@@ -8268,7 +8295,7 @@
         <v>23</v>
       </c>
       <c r="P113" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="Q113" t="s">
         <v>25</v>
@@ -8288,13 +8315,13 @@
         <v>816905</v>
       </c>
       <c r="C114" t="s">
-        <v>19</v>
+        <v>284</v>
       </c>
       <c r="D114" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="E114" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="F114" s="1">
         <v>20</v>
@@ -8306,7 +8333,7 @@
         <v>14</v>
       </c>
       <c r="I114" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J114" s="1">
         <v>13</v>
@@ -8327,7 +8354,7 @@
         <v>23</v>
       </c>
       <c r="P114" t="s">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="Q114" t="s">
         <v>25</v>
@@ -8347,13 +8374,13 @@
         <v>932132</v>
       </c>
       <c r="C115" t="s">
-        <v>19</v>
+        <v>284</v>
       </c>
       <c r="D115" t="s">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="E115" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="F115" s="1">
         <v>20</v>
@@ -8365,7 +8392,7 @@
         <v>14</v>
       </c>
       <c r="I115" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J115" s="1">
         <v>13</v>
@@ -8386,7 +8413,7 @@
         <v>23</v>
       </c>
       <c r="P115" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="Q115" t="s">
         <v>25</v>
@@ -8406,13 +8433,13 @@
         <v>840822</v>
       </c>
       <c r="C116" t="s">
-        <v>19</v>
+        <v>284</v>
       </c>
       <c r="D116" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="E116" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="F116" s="1">
         <v>20</v>
@@ -8424,7 +8451,7 @@
         <v>14</v>
       </c>
       <c r="I116" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J116" s="1">
         <v>13</v>
@@ -8445,7 +8472,7 @@
         <v>23</v>
       </c>
       <c r="P116" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="Q116" t="s">
         <v>25</v>
@@ -8465,13 +8492,13 @@
         <v>900309</v>
       </c>
       <c r="C117" t="s">
-        <v>19</v>
+        <v>284</v>
       </c>
       <c r="D117" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="E117" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="F117" s="1">
         <v>20</v>
@@ -8483,7 +8510,7 @@
         <v>14</v>
       </c>
       <c r="I117" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J117" s="1">
         <v>13</v>
@@ -8504,7 +8531,7 @@
         <v>23</v>
       </c>
       <c r="P117" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="Q117" t="s">
         <v>25</v>
@@ -8524,13 +8551,13 @@
         <v>913653</v>
       </c>
       <c r="C118" t="s">
-        <v>19</v>
+        <v>284</v>
       </c>
       <c r="D118" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="E118" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="F118" s="1">
         <v>15</v>
@@ -8542,7 +8569,7 @@
         <v>13</v>
       </c>
       <c r="I118" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J118" s="1">
         <v>9.75</v>
@@ -8563,7 +8590,7 @@
         <v>23</v>
       </c>
       <c r="P118" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="Q118" t="s">
         <v>25</v>
@@ -8583,13 +8610,13 @@
         <v>818963</v>
       </c>
       <c r="C119" t="s">
-        <v>19</v>
+        <v>284</v>
       </c>
       <c r="D119" t="s">
-        <v>300</v>
+        <v>308</v>
       </c>
       <c r="E119" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="F119" s="1">
         <v>20</v>
@@ -8601,7 +8628,7 @@
         <v>14</v>
       </c>
       <c r="I119" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J119" s="1">
         <v>13</v>
@@ -8622,7 +8649,7 @@
         <v>23</v>
       </c>
       <c r="P119" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="Q119" t="s">
         <v>25</v>
@@ -8642,13 +8669,13 @@
         <v>871143</v>
       </c>
       <c r="C120" t="s">
-        <v>19</v>
+        <v>284</v>
       </c>
       <c r="D120" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="E120" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="F120" s="1">
         <v>20</v>
@@ -8660,7 +8687,7 @@
         <v>14</v>
       </c>
       <c r="I120" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J120" s="1">
         <v>13</v>
@@ -8681,7 +8708,7 @@
         <v>23</v>
       </c>
       <c r="P120" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="Q120" t="s">
         <v>25</v>
@@ -8701,13 +8728,13 @@
         <v>913648</v>
       </c>
       <c r="C121" t="s">
-        <v>19</v>
+        <v>284</v>
       </c>
       <c r="D121" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="E121" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="F121" s="1">
         <v>24</v>
@@ -8719,7 +8746,7 @@
         <v>12</v>
       </c>
       <c r="I121" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J121" s="1">
         <v>15.6</v>
@@ -8740,7 +8767,7 @@
         <v>23</v>
       </c>
       <c r="P121" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="Q121" t="s">
         <v>25</v>
@@ -8760,13 +8787,13 @@
         <v>805663</v>
       </c>
       <c r="C122" t="s">
-        <v>19</v>
+        <v>284</v>
       </c>
       <c r="D122" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="E122" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="F122" s="1">
         <v>20</v>
@@ -8778,7 +8805,7 @@
         <v>16</v>
       </c>
       <c r="I122" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J122" s="1">
         <v>13</v>
@@ -8799,7 +8826,7 @@
         <v>23</v>
       </c>
       <c r="P122" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="Q122" t="s">
         <v>25</v>
@@ -8819,13 +8846,13 @@
         <v>941045</v>
       </c>
       <c r="C123" t="s">
-        <v>19</v>
+        <v>284</v>
       </c>
       <c r="D123" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="E123" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="F123" s="1">
         <v>10</v>
@@ -8837,7 +8864,7 @@
         <v>8</v>
       </c>
       <c r="I123" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J123" s="1">
         <v>6.5</v>
@@ -8858,7 +8885,7 @@
         <v>23</v>
       </c>
       <c r="P123" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="Q123" t="s">
         <v>25</v>
@@ -8878,13 +8905,13 @@
         <v>805651</v>
       </c>
       <c r="C124" t="s">
-        <v>19</v>
+        <v>284</v>
       </c>
       <c r="D124" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="E124" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="F124" s="1">
         <v>15</v>
@@ -8896,7 +8923,7 @@
         <v>16</v>
       </c>
       <c r="I124" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J124" s="1">
         <v>9.75</v>
@@ -8917,7 +8944,7 @@
         <v>23</v>
       </c>
       <c r="P124" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="Q124" t="s">
         <v>25</v>
@@ -8937,13 +8964,13 @@
         <v>941062</v>
       </c>
       <c r="C125" t="s">
-        <v>19</v>
+        <v>284</v>
       </c>
       <c r="D125" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="E125" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="F125" s="1">
         <v>10</v>
@@ -8955,7 +8982,7 @@
         <v>8</v>
       </c>
       <c r="I125" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J125" s="1">
         <v>6.5</v>
@@ -8976,7 +9003,7 @@
         <v>23</v>
       </c>
       <c r="P125" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="Q125" t="s">
         <v>25</v>
@@ -8996,13 +9023,13 @@
         <v>929464</v>
       </c>
       <c r="C126" t="s">
-        <v>19</v>
+        <v>284</v>
       </c>
       <c r="D126" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c r="E126" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="F126" s="1">
         <v>16</v>
@@ -9014,7 +9041,7 @@
         <v>16</v>
       </c>
       <c r="I126" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J126" s="1">
         <v>10.4</v>
@@ -9035,7 +9062,7 @@
         <v>23</v>
       </c>
       <c r="P126" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="Q126" t="s">
         <v>25</v>
@@ -9055,13 +9082,13 @@
         <v>805665</v>
       </c>
       <c r="C127" t="s">
-        <v>19</v>
+        <v>284</v>
       </c>
       <c r="D127" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="E127" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="F127" s="1">
         <v>10</v>
@@ -9073,7 +9100,7 @@
         <v>8</v>
       </c>
       <c r="I127" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J127" s="1">
         <v>6.5</v>
@@ -9094,7 +9121,7 @@
         <v>23</v>
       </c>
       <c r="P127" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="Q127" t="s">
         <v>25</v>
@@ -9114,13 +9141,13 @@
         <v>900310</v>
       </c>
       <c r="C128" t="s">
-        <v>19</v>
+        <v>284</v>
       </c>
       <c r="D128" t="s">
-        <v>316</v>
+        <v>324</v>
       </c>
       <c r="E128" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="F128" s="1">
         <v>22</v>
@@ -9132,7 +9159,7 @@
         <v>14</v>
       </c>
       <c r="I128" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J128" s="1">
         <v>14.3</v>
@@ -9153,7 +9180,7 @@
         <v>23</v>
       </c>
       <c r="P128" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="Q128" t="s">
         <v>25</v>
@@ -9173,13 +9200,13 @@
         <v>913650</v>
       </c>
       <c r="C129" t="s">
-        <v>19</v>
+        <v>284</v>
       </c>
       <c r="D129" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="E129" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="F129" s="1">
         <v>20</v>
@@ -9191,7 +9218,7 @@
         <v>14</v>
       </c>
       <c r="I129" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J129" s="1">
         <v>13</v>
@@ -9212,7 +9239,7 @@
         <v>23</v>
       </c>
       <c r="P129" t="s">
-        <v>319</v>
+        <v>327</v>
       </c>
       <c r="Q129" t="s">
         <v>25</v>
@@ -9232,13 +9259,13 @@
         <v>911651</v>
       </c>
       <c r="C130" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="D130" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
       <c r="E130" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
       <c r="F130" s="1">
         <v>16.6</v>
@@ -9250,7 +9277,7 @@
         <v>0</v>
       </c>
       <c r="I130" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J130" s="1">
         <v>10.79</v>
@@ -9271,7 +9298,7 @@
         <v>25</v>
       </c>
       <c r="P130" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
       <c r="Q130" t="s">
         <v>23</v>
@@ -9291,13 +9318,13 @@
         <v>911647</v>
       </c>
       <c r="C131" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="D131" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="E131" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="F131" s="1">
         <v>20.77</v>
@@ -9309,7 +9336,7 @@
         <v>0</v>
       </c>
       <c r="I131" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J131" s="1">
         <v>13.5</v>
@@ -9330,7 +9357,7 @@
         <v>25</v>
       </c>
       <c r="P131" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
       <c r="Q131" t="s">
         <v>23</v>
@@ -9350,13 +9377,13 @@
         <v>911648</v>
       </c>
       <c r="C132" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="D132" t="s">
-        <v>325</v>
+        <v>334</v>
       </c>
       <c r="E132" t="s">
-        <v>326</v>
+        <v>335</v>
       </c>
       <c r="F132" s="1">
         <v>21.88</v>
@@ -9368,7 +9395,7 @@
         <v>0</v>
       </c>
       <c r="I132" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J132" s="1">
         <v>14.22</v>
@@ -9389,7 +9416,7 @@
         <v>25</v>
       </c>
       <c r="P132" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
       <c r="Q132" t="s">
         <v>23</v>
@@ -9409,13 +9436,13 @@
         <v>957423</v>
       </c>
       <c r="C133" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="D133" t="s">
-        <v>327</v>
+        <v>336</v>
       </c>
       <c r="E133" t="s">
-        <v>328</v>
+        <v>337</v>
       </c>
       <c r="F133" s="1">
         <v>19.23</v>
@@ -9427,7 +9454,7 @@
         <v>0</v>
       </c>
       <c r="I133" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J133" s="1">
         <v>12.5</v>
@@ -9448,7 +9475,7 @@
         <v>25</v>
       </c>
       <c r="P133" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="Q133" t="s">
         <v>23</v>
@@ -9468,13 +9495,13 @@
         <v>957424</v>
       </c>
       <c r="C134" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="D134" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="E134" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="F134" s="1">
         <v>21.88</v>
@@ -9486,7 +9513,7 @@
         <v>0</v>
       </c>
       <c r="I134" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J134" s="1">
         <v>14.22</v>
@@ -9507,7 +9534,7 @@
         <v>25</v>
       </c>
       <c r="P134" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="Q134" t="s">
         <v>23</v>
@@ -9527,13 +9554,13 @@
         <v>936388</v>
       </c>
       <c r="C135" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="D135" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
       <c r="E135" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="F135" s="1">
         <v>16.6</v>
@@ -9545,7 +9572,7 @@
         <v>0</v>
       </c>
       <c r="I135" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J135" s="1">
         <v>10.79</v>
@@ -9566,7 +9593,7 @@
         <v>25</v>
       </c>
       <c r="P135" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
       <c r="Q135" t="s">
         <v>23</v>
@@ -9586,13 +9613,13 @@
         <v>936387</v>
       </c>
       <c r="C136" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="D136" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="E136" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="F136" s="1">
         <v>20.77</v>
@@ -9604,7 +9631,7 @@
         <v>0</v>
       </c>
       <c r="I136" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J136" s="1">
         <v>13.5</v>
@@ -9625,7 +9652,7 @@
         <v>25</v>
       </c>
       <c r="P136" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
       <c r="Q136" t="s">
         <v>23</v>
@@ -9645,13 +9672,13 @@
         <v>824228</v>
       </c>
       <c r="C137" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="D137" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
       <c r="E137" t="s">
-        <v>338</v>
+        <v>347</v>
       </c>
       <c r="F137" s="1">
         <v>21.89</v>
@@ -9663,7 +9690,7 @@
         <v>0</v>
       </c>
       <c r="I137" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J137" s="1">
         <v>14.23</v>
@@ -9684,7 +9711,7 @@
         <v>25</v>
       </c>
       <c r="P137" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
       <c r="Q137" t="s">
         <v>23</v>
@@ -9704,13 +9731,13 @@
         <v>866256</v>
       </c>
       <c r="C138" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="D138" t="s">
-        <v>339</v>
+        <v>348</v>
       </c>
       <c r="E138" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="F138" s="1">
         <v>16.6</v>
@@ -9722,7 +9749,7 @@
         <v>0</v>
       </c>
       <c r="I138" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J138" s="1">
         <v>10.79</v>
@@ -9743,7 +9770,7 @@
         <v>25</v>
       </c>
       <c r="P138" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
       <c r="Q138" t="s">
         <v>23</v>
@@ -9763,13 +9790,13 @@
         <v>805464</v>
       </c>
       <c r="C139" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="D139" t="s">
-        <v>341</v>
+        <v>350</v>
       </c>
       <c r="E139" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="F139" s="1">
         <v>19.23</v>
@@ -9781,7 +9808,7 @@
         <v>0</v>
       </c>
       <c r="I139" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J139" s="1">
         <v>12.5</v>
@@ -9802,7 +9829,7 @@
         <v>25</v>
       </c>
       <c r="P139" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
       <c r="Q139" t="s">
         <v>23</v>
@@ -9822,13 +9849,13 @@
         <v>842611</v>
       </c>
       <c r="C140" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="D140" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="E140" t="s">
-        <v>343</v>
+        <v>352</v>
       </c>
       <c r="F140" s="1">
         <v>21.88</v>
@@ -9840,7 +9867,7 @@
         <v>0</v>
       </c>
       <c r="I140" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J140" s="1">
         <v>14.22</v>
@@ -9861,7 +9888,7 @@
         <v>25</v>
       </c>
       <c r="P140" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
       <c r="Q140" t="s">
         <v>23</v>
@@ -9881,13 +9908,13 @@
         <v>805465</v>
       </c>
       <c r="C141" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="D141" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
       <c r="E141" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F141" s="1">
         <v>15.38</v>
@@ -9899,7 +9926,7 @@
         <v>0</v>
       </c>
       <c r="I141" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J141" s="1">
         <v>10</v>
@@ -9920,7 +9947,7 @@
         <v>25</v>
       </c>
       <c r="P141" t="s">
-        <v>345</v>
+        <v>354</v>
       </c>
       <c r="Q141" t="s">
         <v>23</v>
@@ -9940,13 +9967,13 @@
         <v>990715</v>
       </c>
       <c r="C142" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="D142" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="E142" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="F142" s="1">
         <v>9.23</v>
@@ -9958,7 +9985,7 @@
         <v>0</v>
       </c>
       <c r="I142" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J142" s="1">
         <v>6</v>
@@ -9979,7 +10006,7 @@
         <v>25</v>
       </c>
       <c r="P142" t="s">
-        <v>345</v>
+        <v>354</v>
       </c>
       <c r="Q142" t="s">
         <v>23</v>
@@ -9999,13 +10026,13 @@
         <v>881794</v>
       </c>
       <c r="C143" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="D143" t="s">
-        <v>347</v>
+        <v>356</v>
       </c>
       <c r="E143" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F143" s="1">
         <v>13.85</v>
@@ -10017,7 +10044,7 @@
         <v>0</v>
       </c>
       <c r="I143" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J143" s="1">
         <v>9</v>
@@ -10038,7 +10065,7 @@
         <v>25</v>
       </c>
       <c r="P143" t="s">
-        <v>348</v>
+        <v>357</v>
       </c>
       <c r="Q143" t="s">
         <v>23</v>
@@ -10058,13 +10085,13 @@
         <v>805466</v>
       </c>
       <c r="C144" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="D144" t="s">
-        <v>349</v>
+        <v>358</v>
       </c>
       <c r="E144" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="F144" s="1">
         <v>22.66</v>
@@ -10076,7 +10103,7 @@
         <v>0</v>
       </c>
       <c r="I144" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J144" s="1">
         <v>14.73</v>
@@ -10097,7 +10124,7 @@
         <v>25</v>
       </c>
       <c r="P144" t="s">
-        <v>351</v>
+        <v>360</v>
       </c>
       <c r="Q144" t="s">
         <v>23</v>
@@ -10117,13 +10144,13 @@
         <v>836358</v>
       </c>
       <c r="C145" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="D145" t="s">
-        <v>352</v>
+        <v>361</v>
       </c>
       <c r="E145" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
       <c r="F145" s="1">
         <v>19.23</v>
@@ -10135,7 +10162,7 @@
         <v>0</v>
       </c>
       <c r="I145" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J145" s="1">
         <v>12.5</v>
@@ -10156,7 +10183,7 @@
         <v>25</v>
       </c>
       <c r="P145" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
       <c r="Q145" t="s">
         <v>23</v>
@@ -10176,13 +10203,13 @@
         <v>867239</v>
       </c>
       <c r="C146" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="D146" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="E146" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
       <c r="F146" s="1">
         <v>20.77</v>
@@ -10194,7 +10221,7 @@
         <v>0</v>
       </c>
       <c r="I146" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J146" s="1">
         <v>13.5</v>
@@ -10215,7 +10242,7 @@
         <v>25</v>
       </c>
       <c r="P146" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
       <c r="Q146" t="s">
         <v>23</v>
@@ -10235,13 +10262,13 @@
         <v>805468</v>
       </c>
       <c r="C147" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="D147" t="s">
-        <v>357</v>
+        <v>366</v>
       </c>
       <c r="E147" t="s">
-        <v>358</v>
+        <v>367</v>
       </c>
       <c r="F147" s="1">
         <v>29.62</v>
@@ -10253,7 +10280,7 @@
         <v>0</v>
       </c>
       <c r="I147" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J147" s="1">
         <v>19.25</v>
@@ -10274,7 +10301,7 @@
         <v>25</v>
       </c>
       <c r="P147" t="s">
-        <v>359</v>
+        <v>368</v>
       </c>
       <c r="Q147" t="s">
         <v>23</v>
@@ -10294,13 +10321,13 @@
         <v>805469</v>
       </c>
       <c r="C148" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="D148" t="s">
-        <v>360</v>
+        <v>369</v>
       </c>
       <c r="E148" t="s">
-        <v>361</v>
+        <v>370</v>
       </c>
       <c r="F148" s="1">
         <v>32.69</v>
@@ -10312,7 +10339,7 @@
         <v>0</v>
       </c>
       <c r="I148" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J148" s="1">
         <v>21.25</v>
@@ -10333,7 +10360,7 @@
         <v>25</v>
       </c>
       <c r="P148" t="s">
-        <v>362</v>
+        <v>371</v>
       </c>
       <c r="Q148" t="s">
         <v>23</v>
@@ -10353,13 +10380,13 @@
         <v>805461</v>
       </c>
       <c r="C149" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="D149" t="s">
-        <v>363</v>
+        <v>372</v>
       </c>
       <c r="E149" t="s">
-        <v>364</v>
+        <v>373</v>
       </c>
       <c r="F149" s="1">
         <v>23.08</v>
@@ -10371,7 +10398,7 @@
         <v>0</v>
       </c>
       <c r="I149" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J149" s="1">
         <v>15</v>
@@ -10392,7 +10419,7 @@
         <v>25</v>
       </c>
       <c r="P149" t="s">
-        <v>365</v>
+        <v>374</v>
       </c>
       <c r="Q149" t="s">
         <v>23</v>
@@ -10412,13 +10439,13 @@
         <v>805470</v>
       </c>
       <c r="C150" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="D150" t="s">
-        <v>366</v>
+        <v>375</v>
       </c>
       <c r="E150" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
       <c r="F150" s="1">
         <v>21.54</v>
@@ -10430,7 +10457,7 @@
         <v>0</v>
       </c>
       <c r="I150" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J150" s="1">
         <v>14</v>
@@ -10451,7 +10478,7 @@
         <v>25</v>
       </c>
       <c r="P150" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
       <c r="Q150" t="s">
         <v>23</v>
@@ -10471,13 +10498,13 @@
         <v>805471</v>
       </c>
       <c r="C151" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="D151" t="s">
-        <v>369</v>
+        <v>378</v>
       </c>
       <c r="E151" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F151" s="1">
         <v>16.92</v>
@@ -10489,7 +10516,7 @@
         <v>0</v>
       </c>
       <c r="I151" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J151" s="1">
         <v>11</v>
@@ -10510,7 +10537,7 @@
         <v>25</v>
       </c>
       <c r="P151" t="s">
-        <v>370</v>
+        <v>379</v>
       </c>
       <c r="Q151" t="s">
         <v>23</v>
@@ -10530,13 +10557,13 @@
         <v>805472</v>
       </c>
       <c r="C152" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="D152" t="s">
-        <v>371</v>
+        <v>380</v>
       </c>
       <c r="E152" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="F152" s="1">
         <v>15.38</v>
@@ -10548,7 +10575,7 @@
         <v>0</v>
       </c>
       <c r="I152" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J152" s="1">
         <v>10</v>
@@ -10569,7 +10596,7 @@
         <v>25</v>
       </c>
       <c r="P152" t="s">
-        <v>372</v>
+        <v>381</v>
       </c>
       <c r="Q152" t="s">
         <v>23</v>
@@ -10589,13 +10616,13 @@
         <v>805473</v>
       </c>
       <c r="C153" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="D153" t="s">
-        <v>373</v>
+        <v>382</v>
       </c>
       <c r="E153" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F153" s="1">
         <v>15.38</v>
@@ -10607,7 +10634,7 @@
         <v>0</v>
       </c>
       <c r="I153" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J153" s="1">
         <v>10</v>
@@ -10628,7 +10655,7 @@
         <v>25</v>
       </c>
       <c r="P153" t="s">
-        <v>374</v>
+        <v>383</v>
       </c>
       <c r="Q153" t="s">
         <v>23</v>
@@ -10648,13 +10675,13 @@
         <v>805474</v>
       </c>
       <c r="C154" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="D154" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
       <c r="E154" t="s">
-        <v>364</v>
+        <v>373</v>
       </c>
       <c r="F154" s="1">
         <v>15.38</v>
@@ -10666,7 +10693,7 @@
         <v>0</v>
       </c>
       <c r="I154" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J154" s="1">
         <v>10</v>
@@ -10687,7 +10714,7 @@
         <v>25</v>
       </c>
       <c r="P154" t="s">
-        <v>376</v>
+        <v>385</v>
       </c>
       <c r="Q154" t="s">
         <v>23</v>
@@ -10707,13 +10734,13 @@
         <v>990712</v>
       </c>
       <c r="C155" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="D155" t="s">
-        <v>377</v>
+        <v>386</v>
       </c>
       <c r="E155" t="s">
-        <v>378</v>
+        <v>387</v>
       </c>
       <c r="F155" s="1">
         <v>8.92</v>
@@ -10725,7 +10752,7 @@
         <v>0</v>
       </c>
       <c r="I155" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J155" s="1">
         <v>5.8</v>
@@ -10746,7 +10773,7 @@
         <v>25</v>
       </c>
       <c r="P155" t="s">
-        <v>376</v>
+        <v>385</v>
       </c>
       <c r="Q155" t="s">
         <v>23</v>
@@ -10766,13 +10793,13 @@
         <v>805475</v>
       </c>
       <c r="C156" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="D156" t="s">
-        <v>379</v>
+        <v>388</v>
       </c>
       <c r="E156" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
       <c r="F156" s="1">
         <v>18.46</v>
@@ -10784,7 +10811,7 @@
         <v>0</v>
       </c>
       <c r="I156" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J156" s="1">
         <v>12</v>
@@ -10805,7 +10832,7 @@
         <v>25</v>
       </c>
       <c r="P156" t="s">
-        <v>380</v>
+        <v>389</v>
       </c>
       <c r="Q156" t="s">
         <v>23</v>
@@ -10825,13 +10852,13 @@
         <v>805476</v>
       </c>
       <c r="C157" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="D157" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
       <c r="E157" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F157" s="1">
         <v>10.77</v>
@@ -10843,7 +10870,7 @@
         <v>0</v>
       </c>
       <c r="I157" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J157" s="1">
         <v>7</v>
@@ -10864,7 +10891,7 @@
         <v>25</v>
       </c>
       <c r="P157" t="s">
-        <v>382</v>
+        <v>391</v>
       </c>
       <c r="Q157" t="s">
         <v>23</v>
@@ -10884,13 +10911,13 @@
         <v>805477</v>
       </c>
       <c r="C158" t="s">
-        <v>19</v>
+        <v>328</v>
       </c>
       <c r="D158" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="E158" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="F158" s="1">
         <v>18.46</v>
@@ -10902,7 +10929,7 @@
         <v>0</v>
       </c>
       <c r="I158" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J158" s="1">
         <v>12</v>
@@ -10923,7 +10950,7 @@
         <v>25</v>
       </c>
       <c r="P158" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
       <c r="Q158" t="s">
         <v>23</v>
@@ -10948,10 +10975,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
       <c r="B1" t="s">
-        <v>387</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -10959,7 +10986,7 @@
         <v>0.5412</v>
       </c>
       <c r="B2" t="s">
-        <v>388</v>
+        <v>397</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -10967,7 +10994,7 @@
         <v>0.65</v>
       </c>
       <c r="B3" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -10975,7 +11002,7 @@
         <v>0.6574</v>
       </c>
       <c r="B4" t="s">
-        <v>390</v>
+        <v>399</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -10983,7 +11010,7 @@
         <v>0.9</v>
       </c>
       <c r="B5" t="s">
-        <v>391</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaning up commits... changing guest pricing
</commit_message>
<xml_diff>
--- a/docs/masterPriceList.xlsx
+++ b/docs/masterPriceList.xlsx
@@ -1843,7 +1843,7 @@
         <v>13.01</v>
       </c>
       <c r="M2" s="1">
-        <v>14.91</v>
+        <v>15.07</v>
       </c>
       <c r="N2" t="s">
         <v>19</v>
@@ -1902,7 +1902,7 @@
         <v>13.01</v>
       </c>
       <c r="M3" s="1">
-        <v>14.91</v>
+        <v>15.07</v>
       </c>
       <c r="N3" t="s">
         <v>19</v>
@@ -1961,7 +1961,7 @@
         <v>12.11</v>
       </c>
       <c r="M4" s="1">
-        <v>13.88</v>
+        <v>14.03</v>
       </c>
       <c r="N4">
         <v>1</v>
@@ -2020,7 +2020,7 @@
         <v>13.45</v>
       </c>
       <c r="M5" s="1">
-        <v>15.42</v>
+        <v>15.59</v>
       </c>
       <c r="N5">
         <v>1</v>
@@ -2079,7 +2079,7 @@
         <v>14.8</v>
       </c>
       <c r="M6" s="1">
-        <v>16.97</v>
+        <v>17.15</v>
       </c>
       <c r="N6">
         <v>1</v>
@@ -2138,7 +2138,7 @@
         <v>14.8</v>
       </c>
       <c r="M7" s="1">
-        <v>16.97</v>
+        <v>17.15</v>
       </c>
       <c r="N7">
         <v>1</v>
@@ -2197,7 +2197,7 @@
         <v>17.94</v>
       </c>
       <c r="M8" s="1">
-        <v>20.57</v>
+        <v>20.78</v>
       </c>
       <c r="N8">
         <v>1</v>
@@ -2256,7 +2256,7 @@
         <v>19.37</v>
       </c>
       <c r="M9" s="1">
-        <v>22.21</v>
+        <v>22.44</v>
       </c>
       <c r="N9">
         <v>1</v>
@@ -2315,7 +2315,7 @@
         <v>15.25</v>
       </c>
       <c r="M10" s="1">
-        <v>17.48</v>
+        <v>17.66</v>
       </c>
       <c r="N10">
         <v>1</v>
@@ -2374,7 +2374,7 @@
         <v>10.76</v>
       </c>
       <c r="M11" s="1">
-        <v>12.34</v>
+        <v>12.47</v>
       </c>
       <c r="N11">
         <v>1</v>
@@ -2433,7 +2433,7 @@
         <v>8.97</v>
       </c>
       <c r="M12" s="1">
-        <v>10.28</v>
+        <v>10.39</v>
       </c>
       <c r="N12">
         <v>1</v>
@@ -2492,7 +2492,7 @@
         <v>20.59</v>
       </c>
       <c r="M13" s="1">
-        <v>23.6</v>
+        <v>23.85</v>
       </c>
       <c r="N13">
         <v>1</v>
@@ -2551,7 +2551,7 @@
         <v>23.61</v>
       </c>
       <c r="M14" s="1">
-        <v>27.07</v>
+        <v>27.35</v>
       </c>
       <c r="N14">
         <v>1</v>
@@ -2610,7 +2610,7 @@
         <v>41.93</v>
       </c>
       <c r="M15" s="1">
-        <v>48.07</v>
+        <v>48.58</v>
       </c>
       <c r="N15">
         <v>1</v>
@@ -2669,7 +2669,7 @@
         <v>55.1</v>
       </c>
       <c r="M16" s="1">
-        <v>63.16</v>
+        <v>63.83</v>
       </c>
       <c r="N16">
         <v>1</v>
@@ -2728,7 +2728,7 @@
         <v>41.89</v>
       </c>
       <c r="M17" s="1">
-        <v>48.02</v>
+        <v>48.53</v>
       </c>
       <c r="N17">
         <v>1</v>
@@ -2846,7 +2846,7 @@
         <v>32.52</v>
       </c>
       <c r="M19" s="1">
-        <v>37.28</v>
+        <v>37.67</v>
       </c>
       <c r="N19">
         <v>1</v>
@@ -2905,7 +2905,7 @@
         <v>13.66</v>
       </c>
       <c r="M20" s="1">
-        <v>15.66</v>
+        <v>15.82</v>
       </c>
       <c r="N20">
         <v>1</v>
@@ -2964,7 +2964,7 @@
         <v>23.32</v>
       </c>
       <c r="M21" s="1">
-        <v>26.74</v>
+        <v>27.02</v>
       </c>
       <c r="N21">
         <v>1</v>
@@ -3023,7 +3023,7 @@
         <v>42.61</v>
       </c>
       <c r="M22" s="1">
-        <v>48.84</v>
+        <v>49.36</v>
       </c>
       <c r="N22">
         <v>1</v>
@@ -3082,7 +3082,7 @@
         <v>15.25</v>
       </c>
       <c r="M23" s="1">
-        <v>17.48</v>
+        <v>17.66</v>
       </c>
       <c r="N23">
         <v>1</v>
@@ -3141,7 +3141,7 @@
         <v>22.42</v>
       </c>
       <c r="M24" s="1">
-        <v>25.71</v>
+        <v>25.98</v>
       </c>
       <c r="N24">
         <v>1</v>
@@ -3200,7 +3200,7 @@
         <v>12.56</v>
       </c>
       <c r="M25" s="1">
-        <v>14.4</v>
+        <v>14.55</v>
       </c>
       <c r="N25">
         <v>1</v>
@@ -3259,7 +3259,7 @@
         <v>29.15</v>
       </c>
       <c r="M26" s="1">
-        <v>33.42</v>
+        <v>33.77</v>
       </c>
       <c r="N26">
         <v>1</v>
@@ -3318,7 +3318,7 @@
         <v>48.8</v>
       </c>
       <c r="M27" s="1">
-        <v>55.94</v>
+        <v>56.53</v>
       </c>
       <c r="N27">
         <v>1</v>
@@ -3377,7 +3377,7 @@
         <v>9.87</v>
       </c>
       <c r="M28" s="1">
-        <v>11.31</v>
+        <v>11.43</v>
       </c>
       <c r="N28">
         <v>1</v>
@@ -3436,7 +3436,7 @@
         <v>20.99</v>
       </c>
       <c r="M29" s="1">
-        <v>24.06</v>
+        <v>24.32</v>
       </c>
       <c r="N29">
         <v>1</v>
@@ -3495,7 +3495,7 @@
         <v>25.56</v>
       </c>
       <c r="M30" s="1">
-        <v>29.31</v>
+        <v>29.61</v>
       </c>
       <c r="N30">
         <v>1</v>
@@ -3554,7 +3554,7 @@
         <v>20.99</v>
       </c>
       <c r="M31" s="1">
-        <v>24.06</v>
+        <v>24.32</v>
       </c>
       <c r="N31">
         <v>1</v>
@@ -3613,7 +3613,7 @@
         <v>25.65</v>
       </c>
       <c r="M32" s="1">
-        <v>29.41</v>
+        <v>29.72</v>
       </c>
       <c r="N32">
         <v>1</v>
@@ -3672,7 +3672,7 @@
         <v>13.45</v>
       </c>
       <c r="M33" s="1">
-        <v>15.42</v>
+        <v>15.59</v>
       </c>
       <c r="N33">
         <v>1</v>
@@ -3731,7 +3731,7 @@
         <v>19.24</v>
       </c>
       <c r="M34" s="1">
-        <v>22.06</v>
+        <v>22.29</v>
       </c>
       <c r="N34">
         <v>1</v>
@@ -3790,7 +3790,7 @@
         <v>39.36</v>
       </c>
       <c r="M35" s="1">
-        <v>45.12</v>
+        <v>45.59</v>
       </c>
       <c r="N35">
         <v>1</v>
@@ -3849,7 +3849,7 @@
         <v>29.74</v>
       </c>
       <c r="M36" s="1">
-        <v>34.09</v>
+        <v>34.45</v>
       </c>
       <c r="N36">
         <v>1</v>
@@ -3967,7 +3967,7 @@
         <v>19.91</v>
       </c>
       <c r="M38" s="1">
-        <v>22.83</v>
+        <v>23.07</v>
       </c>
       <c r="N38">
         <v>1</v>
@@ -4026,7 +4026,7 @@
         <v>21.21</v>
       </c>
       <c r="M39" s="1">
-        <v>24.32</v>
+        <v>24.57</v>
       </c>
       <c r="N39">
         <v>1</v>
@@ -4085,7 +4085,7 @@
         <v>23.43</v>
       </c>
       <c r="M40" s="1">
-        <v>26.86</v>
+        <v>27.15</v>
       </c>
       <c r="N40">
         <v>1</v>
@@ -4144,7 +4144,7 @@
         <v>38.62</v>
       </c>
       <c r="M41" s="1">
-        <v>44.27</v>
+        <v>44.73</v>
       </c>
       <c r="N41">
         <v>1</v>
@@ -4203,7 +4203,7 @@
         <v>64.58</v>
       </c>
       <c r="M42" s="1">
-        <v>74.04</v>
+        <v>74.82</v>
       </c>
       <c r="N42">
         <v>1</v>
@@ -4262,7 +4262,7 @@
         <v>53.29</v>
       </c>
       <c r="M43" s="1">
-        <v>61.1</v>
+        <v>61.74</v>
       </c>
       <c r="N43">
         <v>1</v>
@@ -4321,7 +4321,7 @@
         <v>42.71</v>
       </c>
       <c r="M44" s="1">
-        <v>48.96</v>
+        <v>49.47</v>
       </c>
       <c r="N44">
         <v>1</v>
@@ -4380,7 +4380,7 @@
         <v>37.31</v>
       </c>
       <c r="M45" s="1">
-        <v>42.78</v>
+        <v>43.23</v>
       </c>
       <c r="N45">
         <v>1</v>
@@ -4439,7 +4439,7 @@
         <v>29.15</v>
       </c>
       <c r="M46" s="1">
-        <v>33.42</v>
+        <v>33.77</v>
       </c>
       <c r="N46">
         <v>1</v>
@@ -4498,7 +4498,7 @@
         <v>13.9</v>
       </c>
       <c r="M47" s="1">
-        <v>15.94</v>
+        <v>16.11</v>
       </c>
       <c r="N47">
         <v>1</v>
@@ -4557,7 +4557,7 @@
         <v>12.83</v>
       </c>
       <c r="M48" s="1">
-        <v>14.7</v>
+        <v>14.86</v>
       </c>
       <c r="N48">
         <v>1</v>
@@ -4616,7 +4616,7 @@
         <v>22.74</v>
       </c>
       <c r="M49" s="1">
-        <v>26.07</v>
+        <v>26.34</v>
       </c>
       <c r="N49">
         <v>1</v>
@@ -4675,7 +4675,7 @@
         <v>10.76</v>
       </c>
       <c r="M50" s="1">
-        <v>12.34</v>
+        <v>12.47</v>
       </c>
       <c r="N50">
         <v>1</v>
@@ -4734,7 +4734,7 @@
         <v>23.23</v>
       </c>
       <c r="M51" s="1">
-        <v>26.63</v>
+        <v>26.91</v>
       </c>
       <c r="N51">
         <v>1</v>
@@ -4793,7 +4793,7 @@
         <v>10.76</v>
       </c>
       <c r="M52" s="1">
-        <v>12.34</v>
+        <v>12.47</v>
       </c>
       <c r="N52">
         <v>1</v>
@@ -4852,7 +4852,7 @@
         <v>34.51</v>
       </c>
       <c r="M53" s="1">
-        <v>39.56</v>
+        <v>39.98</v>
       </c>
       <c r="N53">
         <v>1</v>
@@ -4911,7 +4911,7 @@
         <v>23.32</v>
       </c>
       <c r="M54" s="1">
-        <v>26.74</v>
+        <v>27.02</v>
       </c>
       <c r="N54">
         <v>1</v>
@@ -4970,7 +4970,7 @@
         <v>13.88</v>
       </c>
       <c r="M55" s="1">
-        <v>15.91</v>
+        <v>16.07</v>
       </c>
       <c r="N55">
         <v>1</v>
@@ -5029,7 +5029,7 @@
         <v>12.83</v>
       </c>
       <c r="M56" s="1">
-        <v>14.7</v>
+        <v>14.86</v>
       </c>
       <c r="N56">
         <v>1</v>
@@ -5088,7 +5088,7 @@
         <v>32.52</v>
       </c>
       <c r="M57" s="1">
-        <v>37.28</v>
+        <v>37.67</v>
       </c>
       <c r="N57">
         <v>1</v>
@@ -5147,7 +5147,7 @@
         <v>12.78</v>
       </c>
       <c r="M58" s="1">
-        <v>14.65</v>
+        <v>14.81</v>
       </c>
       <c r="N58">
         <v>1</v>
@@ -5206,7 +5206,7 @@
         <v>8.52</v>
       </c>
       <c r="M59" s="1">
-        <v>9.77</v>
+        <v>9.87</v>
       </c>
       <c r="N59">
         <v>1</v>
@@ -5265,7 +5265,7 @@
         <v>8.52</v>
       </c>
       <c r="M60" s="1">
-        <v>9.77</v>
+        <v>9.87</v>
       </c>
       <c r="N60">
         <v>1</v>
@@ -5324,7 +5324,7 @@
         <v>10.76</v>
       </c>
       <c r="M61" s="1">
-        <v>12.34</v>
+        <v>12.47</v>
       </c>
       <c r="N61">
         <v>1</v>
@@ -5383,7 +5383,7 @@
         <v>24.22</v>
       </c>
       <c r="M62" s="1">
-        <v>27.76</v>
+        <v>28.06</v>
       </c>
       <c r="N62">
         <v>1</v>
@@ -5442,7 +5442,7 @@
         <v>17.38</v>
       </c>
       <c r="M63" s="1">
-        <v>19.92</v>
+        <v>20.13</v>
       </c>
       <c r="N63">
         <v>1</v>
@@ -5501,7 +5501,7 @@
         <v>18.84</v>
       </c>
       <c r="M64" s="1">
-        <v>21.59</v>
+        <v>21.82</v>
       </c>
       <c r="N64">
         <v>1</v>
@@ -5560,7 +5560,7 @@
         <v>44.4</v>
       </c>
       <c r="M65" s="1">
-        <v>50.9</v>
+        <v>51.44</v>
       </c>
       <c r="N65">
         <v>1</v>
@@ -5619,7 +5619,7 @@
         <v>39.2</v>
       </c>
       <c r="M66" s="1">
-        <v>44.94</v>
+        <v>45.41</v>
       </c>
       <c r="N66">
         <v>1</v>
@@ -5678,7 +5678,7 @@
         <v>33.19</v>
       </c>
       <c r="M67" s="1">
-        <v>38.05</v>
+        <v>38.45</v>
       </c>
       <c r="N67">
         <v>1</v>
@@ -5737,7 +5737,7 @@
         <v>26.8</v>
       </c>
       <c r="M68" s="1">
-        <v>30.72</v>
+        <v>31.04</v>
       </c>
       <c r="N68">
         <v>1</v>
@@ -5796,7 +5796,7 @@
         <v>57.64</v>
       </c>
       <c r="M69" s="1">
-        <v>66.08</v>
+        <v>66.77</v>
       </c>
       <c r="N69">
         <v>1</v>
@@ -5855,7 +5855,7 @@
         <v>48.49</v>
       </c>
       <c r="M70" s="1">
-        <v>55.59</v>
+        <v>56.17</v>
       </c>
       <c r="N70">
         <v>1</v>
@@ -5914,7 +5914,7 @@
         <v>37.67</v>
       </c>
       <c r="M71" s="1">
-        <v>43.19</v>
+        <v>43.64</v>
       </c>
       <c r="N71">
         <v>1</v>
@@ -5973,7 +5973,7 @@
         <v>16.59</v>
       </c>
       <c r="M72" s="1">
-        <v>19.02</v>
+        <v>19.22</v>
       </c>
       <c r="N72">
         <v>1</v>
@@ -6032,7 +6032,7 @@
         <v>10.76</v>
       </c>
       <c r="M73" s="1">
-        <v>12.34</v>
+        <v>12.47</v>
       </c>
       <c r="N73">
         <v>1</v>
@@ -6091,7 +6091,7 @@
         <v>17.94</v>
       </c>
       <c r="M74" s="1">
-        <v>20.57</v>
+        <v>20.78</v>
       </c>
       <c r="N74">
         <v>1</v>
@@ -6150,7 +6150,7 @@
         <v>8.97</v>
       </c>
       <c r="M75" s="1">
-        <v>10.28</v>
+        <v>10.39</v>
       </c>
       <c r="N75">
         <v>1</v>
@@ -6209,7 +6209,7 @@
         <v>19.37</v>
       </c>
       <c r="M76" s="1">
-        <v>22.21</v>
+        <v>22.44</v>
       </c>
       <c r="N76">
         <v>1</v>
@@ -6268,7 +6268,7 @@
         <v>37.67</v>
       </c>
       <c r="M77" s="1">
-        <v>43.19</v>
+        <v>43.64</v>
       </c>
       <c r="N77">
         <v>1</v>
@@ -6327,7 +6327,7 @@
         <v>8.1</v>
       </c>
       <c r="M78" s="1">
-        <v>9.28</v>
+        <v>9.38</v>
       </c>
       <c r="N78">
         <v>1</v>
@@ -6386,7 +6386,7 @@
         <v>23.62</v>
       </c>
       <c r="M79" s="1">
-        <v>27.08</v>
+        <v>27.37</v>
       </c>
       <c r="N79">
         <v>1</v>
@@ -6445,7 +6445,7 @@
         <v>18.07</v>
       </c>
       <c r="M80" s="1">
-        <v>20.72</v>
+        <v>20.94</v>
       </c>
       <c r="N80">
         <v>1</v>
@@ -6504,7 +6504,7 @@
         <v>27.38</v>
       </c>
       <c r="M81" s="1">
-        <v>31.39</v>
+        <v>31.72</v>
       </c>
       <c r="N81">
         <v>1</v>
@@ -6563,7 +6563,7 @@
         <v>21.3</v>
       </c>
       <c r="M82" s="1">
-        <v>24.42</v>
+        <v>24.68</v>
       </c>
       <c r="N82">
         <v>1</v>
@@ -6622,7 +6622,7 @@
         <v>38.35</v>
       </c>
       <c r="M83" s="1">
-        <v>43.96</v>
+        <v>44.42</v>
       </c>
       <c r="N83">
         <v>1</v>
@@ -6681,7 +6681,7 @@
         <v>44.85</v>
       </c>
       <c r="M84" s="1">
-        <v>51.41</v>
+        <v>51.96</v>
       </c>
       <c r="N84">
         <v>1</v>
@@ -6799,7 +6799,7 @@
         <v>19.29</v>
       </c>
       <c r="M86" s="1">
-        <v>22.11</v>
+        <v>22.34</v>
       </c>
       <c r="N86">
         <v>1</v>
@@ -6858,7 +6858,7 @@
         <v>54</v>
       </c>
       <c r="M87" s="1">
-        <v>61.9</v>
+        <v>62.55</v>
       </c>
       <c r="N87">
         <v>1</v>
@@ -6917,7 +6917,7 @@
         <v>13.01</v>
       </c>
       <c r="M88" s="1">
-        <v>14.91</v>
+        <v>15.07</v>
       </c>
       <c r="N88">
         <v>1</v>
@@ -6976,7 +6976,7 @@
         <v>15.7</v>
       </c>
       <c r="M89" s="1">
-        <v>17.99</v>
+        <v>18.18</v>
       </c>
       <c r="N89">
         <v>1</v>
@@ -7035,7 +7035,7 @@
         <v>17.49</v>
       </c>
       <c r="M90" s="1">
-        <v>20.05</v>
+        <v>20.26</v>
       </c>
       <c r="N90">
         <v>1</v>
@@ -7094,7 +7094,7 @@
         <v>13.9</v>
       </c>
       <c r="M91" s="1">
-        <v>15.94</v>
+        <v>16.11</v>
       </c>
       <c r="N91">
         <v>1</v>
@@ -7153,7 +7153,7 @@
         <v>17.49</v>
       </c>
       <c r="M92" s="1">
-        <v>20.05</v>
+        <v>20.26</v>
       </c>
       <c r="N92">
         <v>1</v>
@@ -7212,7 +7212,7 @@
         <v>17.49</v>
       </c>
       <c r="M93" s="1">
-        <v>20.05</v>
+        <v>20.26</v>
       </c>
       <c r="N93">
         <v>1</v>
@@ -7271,7 +7271,7 @@
         <v>19.29</v>
       </c>
       <c r="M94" s="1">
-        <v>22.11</v>
+        <v>22.34</v>
       </c>
       <c r="N94">
         <v>1</v>
@@ -7330,7 +7330,7 @@
         <v>19.29</v>
       </c>
       <c r="M95" s="1">
-        <v>22.11</v>
+        <v>22.34</v>
       </c>
       <c r="N95">
         <v>1</v>
@@ -7389,7 +7389,7 @@
         <v>14.8</v>
       </c>
       <c r="M96" s="1">
-        <v>16.97</v>
+        <v>17.15</v>
       </c>
       <c r="N96">
         <v>1</v>
@@ -7448,7 +7448,7 @@
         <v>17.94</v>
       </c>
       <c r="M97" s="1">
-        <v>20.57</v>
+        <v>20.78</v>
       </c>
       <c r="N97">
         <v>1</v>
@@ -7507,7 +7507,7 @@
         <v>19.29</v>
       </c>
       <c r="M98" s="1">
-        <v>22.11</v>
+        <v>22.34</v>
       </c>
       <c r="N98">
         <v>1</v>
@@ -7566,7 +7566,7 @@
         <v>16.15</v>
       </c>
       <c r="M99" s="1">
-        <v>18.51</v>
+        <v>18.7</v>
       </c>
       <c r="N99">
         <v>1</v>
@@ -7625,7 +7625,7 @@
         <v>16.15</v>
       </c>
       <c r="M100" s="1">
-        <v>18.51</v>
+        <v>18.7</v>
       </c>
       <c r="N100">
         <v>1</v>
@@ -7684,7 +7684,7 @@
         <v>17.94</v>
       </c>
       <c r="M101" s="1">
-        <v>20.57</v>
+        <v>20.78</v>
       </c>
       <c r="N101">
         <v>1</v>
@@ -7743,7 +7743,7 @@
         <v>16.15</v>
       </c>
       <c r="M102" s="1">
-        <v>18.51</v>
+        <v>18.7</v>
       </c>
       <c r="N102">
         <v>1</v>
@@ -7802,7 +7802,7 @@
         <v>17.94</v>
       </c>
       <c r="M103" s="1">
-        <v>20.57</v>
+        <v>20.78</v>
       </c>
       <c r="N103">
         <v>1</v>
@@ -7861,7 +7861,7 @@
         <v>8.07</v>
       </c>
       <c r="M104" s="1">
-        <v>9.25</v>
+        <v>9.35</v>
       </c>
       <c r="N104">
         <v>1</v>
@@ -7920,7 +7920,7 @@
         <v>17.49</v>
       </c>
       <c r="M105" s="1">
-        <v>20.05</v>
+        <v>20.26</v>
       </c>
       <c r="N105">
         <v>1</v>
@@ -7979,7 +7979,7 @@
         <v>17.94</v>
       </c>
       <c r="M106" s="1">
-        <v>20.57</v>
+        <v>20.78</v>
       </c>
       <c r="N106">
         <v>1</v>
@@ -8038,7 +8038,7 @@
         <v>14.8</v>
       </c>
       <c r="M107" s="1">
-        <v>16.97</v>
+        <v>17.15</v>
       </c>
       <c r="N107">
         <v>1</v>
@@ -8097,7 +8097,7 @@
         <v>9.87</v>
       </c>
       <c r="M108" s="1">
-        <v>11.31</v>
+        <v>11.43</v>
       </c>
       <c r="N108">
         <v>1</v>
@@ -8156,7 +8156,7 @@
         <v>15.25</v>
       </c>
       <c r="M109" s="1">
-        <v>17.48</v>
+        <v>17.66</v>
       </c>
       <c r="N109">
         <v>1</v>
@@ -8215,7 +8215,7 @@
         <v>17.49</v>
       </c>
       <c r="M110" s="1">
-        <v>20.05</v>
+        <v>20.26</v>
       </c>
       <c r="N110">
         <v>1</v>
@@ -8274,7 +8274,7 @@
         <v>16.15</v>
       </c>
       <c r="M111" s="1">
-        <v>18.51</v>
+        <v>18.7</v>
       </c>
       <c r="N111">
         <v>1</v>
@@ -8333,7 +8333,7 @@
         <v>10.76</v>
       </c>
       <c r="M112" s="1">
-        <v>12.34</v>
+        <v>12.47</v>
       </c>
       <c r="N112">
         <v>1</v>
@@ -8392,7 +8392,7 @@
         <v>6.28</v>
       </c>
       <c r="M113" s="1">
-        <v>7.2</v>
+        <v>7.27</v>
       </c>
       <c r="N113">
         <v>1</v>
@@ -8451,7 +8451,7 @@
         <v>8.97</v>
       </c>
       <c r="M114" s="1">
-        <v>10.28</v>
+        <v>10.39</v>
       </c>
       <c r="N114">
         <v>1</v>
@@ -8510,7 +8510,7 @@
         <v>17.94</v>
       </c>
       <c r="M115" s="1">
-        <v>20.57</v>
+        <v>20.78</v>
       </c>
       <c r="N115">
         <v>1</v>
@@ -8569,7 +8569,7 @@
         <v>14.8</v>
       </c>
       <c r="M116" s="1">
-        <v>16.97</v>
+        <v>17.15</v>
       </c>
       <c r="N116">
         <v>1</v>
@@ -8628,7 +8628,7 @@
         <v>14.8</v>
       </c>
       <c r="M117" s="1">
-        <v>16.97</v>
+        <v>17.15</v>
       </c>
       <c r="N117">
         <v>1</v>
@@ -8687,7 +8687,7 @@
         <v>14.8</v>
       </c>
       <c r="M118" s="1">
-        <v>16.97</v>
+        <v>17.15</v>
       </c>
       <c r="N118">
         <v>1</v>
@@ -8746,7 +8746,7 @@
         <v>15.25</v>
       </c>
       <c r="M119" s="1">
-        <v>17.48</v>
+        <v>17.66</v>
       </c>
       <c r="N119">
         <v>1</v>
@@ -8805,7 +8805,7 @@
         <v>14.8</v>
       </c>
       <c r="M120" s="1">
-        <v>16.97</v>
+        <v>17.15</v>
       </c>
       <c r="N120">
         <v>1</v>
@@ -8864,7 +8864,7 @@
         <v>17.94</v>
       </c>
       <c r="M121" s="1">
-        <v>20.57</v>
+        <v>20.78</v>
       </c>
       <c r="N121">
         <v>1</v>
@@ -8923,7 +8923,7 @@
         <v>17.94</v>
       </c>
       <c r="M122" s="1">
-        <v>20.57</v>
+        <v>20.78</v>
       </c>
       <c r="N122">
         <v>1</v>
@@ -8982,7 +8982,7 @@
         <v>17.94</v>
       </c>
       <c r="M123" s="1">
-        <v>20.57</v>
+        <v>20.78</v>
       </c>
       <c r="N123">
         <v>1</v>
@@ -9041,7 +9041,7 @@
         <v>13.45</v>
       </c>
       <c r="M124" s="1">
-        <v>15.42</v>
+        <v>15.59</v>
       </c>
       <c r="N124">
         <v>1</v>
@@ -9100,7 +9100,7 @@
         <v>17.94</v>
       </c>
       <c r="M125" s="1">
-        <v>20.57</v>
+        <v>20.78</v>
       </c>
       <c r="N125">
         <v>1</v>
@@ -9159,7 +9159,7 @@
         <v>17.94</v>
       </c>
       <c r="M126" s="1">
-        <v>20.57</v>
+        <v>20.78</v>
       </c>
       <c r="N126">
         <v>1</v>
@@ -9218,7 +9218,7 @@
         <v>21.53</v>
       </c>
       <c r="M127" s="1">
-        <v>24.68</v>
+        <v>24.94</v>
       </c>
       <c r="N127">
         <v>1</v>
@@ -9277,7 +9277,7 @@
         <v>17.94</v>
       </c>
       <c r="M128" s="1">
-        <v>20.57</v>
+        <v>20.78</v>
       </c>
       <c r="N128">
         <v>1</v>
@@ -9336,7 +9336,7 @@
         <v>8.97</v>
       </c>
       <c r="M129" s="1">
-        <v>10.28</v>
+        <v>10.39</v>
       </c>
       <c r="N129">
         <v>1</v>
@@ -9395,7 +9395,7 @@
         <v>13.45</v>
       </c>
       <c r="M130" s="1">
-        <v>15.42</v>
+        <v>15.59</v>
       </c>
       <c r="N130">
         <v>1</v>
@@ -9454,7 +9454,7 @@
         <v>8.97</v>
       </c>
       <c r="M131" s="1">
-        <v>10.28</v>
+        <v>10.39</v>
       </c>
       <c r="N131">
         <v>1</v>
@@ -9513,7 +9513,7 @@
         <v>14.35</v>
       </c>
       <c r="M132" s="1">
-        <v>16.45</v>
+        <v>16.63</v>
       </c>
       <c r="N132">
         <v>1</v>
@@ -9572,7 +9572,7 @@
         <v>8.97</v>
       </c>
       <c r="M133" s="1">
-        <v>10.28</v>
+        <v>10.39</v>
       </c>
       <c r="N133">
         <v>1</v>
@@ -9631,7 +9631,7 @@
         <v>19.73</v>
       </c>
       <c r="M134" s="1">
-        <v>22.62</v>
+        <v>22.86</v>
       </c>
       <c r="N134">
         <v>1</v>
@@ -9690,7 +9690,7 @@
         <v>17.94</v>
       </c>
       <c r="M135" s="1">
-        <v>20.57</v>
+        <v>20.78</v>
       </c>
       <c r="N135">
         <v>1</v>
@@ -9749,7 +9749,7 @@
         <v>14.89</v>
       </c>
       <c r="M136" s="1">
-        <v>17.07</v>
+        <v>17.25</v>
       </c>
       <c r="N136">
         <v>1</v>
@@ -9808,7 +9808,7 @@
         <v>18.63</v>
       </c>
       <c r="M137" s="1">
-        <v>21.36</v>
+        <v>21.58</v>
       </c>
       <c r="N137">
         <v>1</v>
@@ -9867,7 +9867,7 @@
         <v>19.63</v>
       </c>
       <c r="M138" s="1">
-        <v>22.5</v>
+        <v>22.74</v>
       </c>
       <c r="N138">
         <v>1</v>
@@ -9926,7 +9926,7 @@
         <v>17.25</v>
       </c>
       <c r="M139" s="1">
-        <v>19.77</v>
+        <v>19.98</v>
       </c>
       <c r="N139">
         <v>1</v>
@@ -9985,7 +9985,7 @@
         <v>19.63</v>
       </c>
       <c r="M140" s="1">
-        <v>22.5</v>
+        <v>22.74</v>
       </c>
       <c r="N140">
         <v>1</v>
@@ -10044,7 +10044,7 @@
         <v>14.89</v>
       </c>
       <c r="M141" s="1">
-        <v>17.07</v>
+        <v>17.25</v>
       </c>
       <c r="N141">
         <v>1</v>
@@ -10103,7 +10103,7 @@
         <v>18.63</v>
       </c>
       <c r="M142" s="1">
-        <v>21.36</v>
+        <v>21.58</v>
       </c>
       <c r="N142">
         <v>1</v>
@@ -10162,7 +10162,7 @@
         <v>19.63</v>
       </c>
       <c r="M143" s="1">
-        <v>22.51</v>
+        <v>22.75</v>
       </c>
       <c r="N143">
         <v>1</v>
@@ -10221,7 +10221,7 @@
         <v>14.89</v>
       </c>
       <c r="M144" s="1">
-        <v>17.07</v>
+        <v>17.25</v>
       </c>
       <c r="N144">
         <v>1</v>
@@ -10280,7 +10280,7 @@
         <v>17.25</v>
       </c>
       <c r="M145" s="1">
-        <v>19.77</v>
+        <v>19.98</v>
       </c>
       <c r="N145">
         <v>1</v>
@@ -10339,7 +10339,7 @@
         <v>19.63</v>
       </c>
       <c r="M146" s="1">
-        <v>22.5</v>
+        <v>22.74</v>
       </c>
       <c r="N146">
         <v>1</v>
@@ -10398,7 +10398,7 @@
         <v>13.8</v>
       </c>
       <c r="M147" s="1">
-        <v>15.81</v>
+        <v>15.98</v>
       </c>
       <c r="N147">
         <v>1</v>
@@ -10457,7 +10457,7 @@
         <v>8.28</v>
       </c>
       <c r="M148" s="1">
-        <v>9.49</v>
+        <v>9.59</v>
       </c>
       <c r="N148">
         <v>1</v>
@@ -10516,7 +10516,7 @@
         <v>12.42</v>
       </c>
       <c r="M149" s="1">
-        <v>14.24</v>
+        <v>14.39</v>
       </c>
       <c r="N149">
         <v>1</v>
@@ -10575,7 +10575,7 @@
         <v>20.33</v>
       </c>
       <c r="M150" s="1">
-        <v>23.3</v>
+        <v>23.55</v>
       </c>
       <c r="N150">
         <v>1</v>
@@ -10634,7 +10634,7 @@
         <v>17.25</v>
       </c>
       <c r="M151" s="1">
-        <v>19.77</v>
+        <v>19.98</v>
       </c>
       <c r="N151">
         <v>1</v>
@@ -10693,7 +10693,7 @@
         <v>18.63</v>
       </c>
       <c r="M152" s="1">
-        <v>21.36</v>
+        <v>21.58</v>
       </c>
       <c r="N152">
         <v>1</v>
@@ -10752,7 +10752,7 @@
         <v>26.57</v>
       </c>
       <c r="M153" s="1">
-        <v>30.46</v>
+        <v>30.78</v>
       </c>
       <c r="N153">
         <v>1</v>
@@ -10811,7 +10811,7 @@
         <v>29.32</v>
       </c>
       <c r="M154" s="1">
-        <v>33.61</v>
+        <v>33.97</v>
       </c>
       <c r="N154">
         <v>1</v>
@@ -10870,7 +10870,7 @@
         <v>20.7</v>
       </c>
       <c r="M155" s="1">
-        <v>23.73</v>
+        <v>23.98</v>
       </c>
       <c r="N155">
         <v>1</v>
@@ -10929,7 +10929,7 @@
         <v>19.32</v>
       </c>
       <c r="M156" s="1">
-        <v>22.15</v>
+        <v>22.38</v>
       </c>
       <c r="N156">
         <v>1</v>
@@ -10988,7 +10988,7 @@
         <v>15.18</v>
       </c>
       <c r="M157" s="1">
-        <v>17.4</v>
+        <v>17.58</v>
       </c>
       <c r="N157">
         <v>1</v>
@@ -11047,7 +11047,7 @@
         <v>13.8</v>
       </c>
       <c r="M158" s="1">
-        <v>15.81</v>
+        <v>15.98</v>
       </c>
       <c r="N158">
         <v>1</v>
@@ -11106,7 +11106,7 @@
         <v>13.8</v>
       </c>
       <c r="M159" s="1">
-        <v>15.81</v>
+        <v>15.98</v>
       </c>
       <c r="N159">
         <v>1</v>
@@ -11165,7 +11165,7 @@
         <v>13.8</v>
       </c>
       <c r="M160" s="1">
-        <v>15.81</v>
+        <v>15.98</v>
       </c>
       <c r="N160">
         <v>1</v>
@@ -11224,7 +11224,7 @@
         <v>8</v>
       </c>
       <c r="M161" s="1">
-        <v>9.17</v>
+        <v>9.27</v>
       </c>
       <c r="N161">
         <v>1</v>
@@ -11283,7 +11283,7 @@
         <v>16.56</v>
       </c>
       <c r="M162" s="1">
-        <v>18.98</v>
+        <v>19.18</v>
       </c>
       <c r="N162">
         <v>1</v>
@@ -11342,7 +11342,7 @@
         <v>9.66</v>
       </c>
       <c r="M163" s="1">
-        <v>11.07</v>
+        <v>11.19</v>
       </c>
       <c r="N163">
         <v>1</v>
@@ -11401,7 +11401,7 @@
         <v>16.56</v>
       </c>
       <c r="M164" s="1">
-        <v>18.98</v>
+        <v>19.18</v>
       </c>
       <c r="N164">
         <v>1</v>
@@ -11467,7 +11467,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>0.9</v>
+        <v>0.92</v>
       </c>
       <c r="B5" t="s">
         <v>429</v>

</xml_diff>